<commit_message>
incorporate nh4no3, add correlation matrices, and start improving data exploration
</commit_message>
<xml_diff>
--- a/data/sources_list_.xlsx
+++ b/data/sources_list_.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clara/Downloads/RE_ ML for AWH Discussion/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clara/Downloads/RE_ ML for AWH Discussion/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05574BA-7250-194C-98E2-EECD58201236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1905FFE-40A5-1548-B975-09D0200E2583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12380" yWindow="760" windowWidth="17860" windowHeight="17840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="400">
   <si>
     <t xml:space="preserve">Data Source </t>
   </si>
@@ -1221,13 +1221,28 @@
   </si>
   <si>
     <t>Paper 18 (BaBr2)</t>
+  </si>
+  <si>
+    <t>NH4NO3</t>
+  </si>
+  <si>
+    <t>Used by Garin</t>
+  </si>
+  <si>
+    <t>Deliquescence, Efflorescence, and Water Activity in Ammonium Nitrate and Mixed</t>
+  </si>
+  <si>
+    <t>Paper 19 (NH4NO3)</t>
+  </si>
+  <si>
+    <t>mole ratio (water:salt)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1263,6 +1278,13 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1291,7 +1313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1316,6 +1338,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2786,10 +2811,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:HY34"/>
+  <dimension ref="A1:IC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HT9" zoomScale="143" workbookViewId="0">
-      <selection activeCell="HX16" sqref="HX16"/>
+    <sheetView tabSelected="1" topLeftCell="HX3" zoomScale="143" workbookViewId="0">
+      <selection activeCell="IA11" sqref="IA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="49" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2825,7 +2850,7 @@
     <col min="345" max="16384" width="20.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:233" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:237" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>136</v>
       </c>
@@ -2944,6 +2969,9 @@
       <c r="AZ1" s="8" t="s">
         <v>380</v>
       </c>
+      <c r="BA1" s="8" t="s">
+        <v>395</v>
+      </c>
       <c r="BC1" s="4" t="s">
         <v>161</v>
       </c>
@@ -3008,7 +3036,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>90</v>
       </c>
@@ -3147,6 +3175,9 @@
       <c r="AZ2" s="2">
         <v>297.14</v>
       </c>
+      <c r="BA2" s="2">
+        <v>80.043000000000006</v>
+      </c>
       <c r="BD2" s="2" t="s">
         <v>166</v>
       </c>
@@ -3196,7 +3227,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>178</v>
       </c>
@@ -3365,8 +3396,12 @@
         <v>0.20823</v>
       </c>
       <c r="AZ3" s="2">
-        <f t="shared" ref="AZ3" si="13">AZ2/1000</f>
+        <f t="shared" ref="AZ3:BA3" si="13">AZ2/1000</f>
         <v>0.29713999999999996</v>
+      </c>
+      <c r="BA3" s="2">
+        <f t="shared" si="13"/>
+        <v>8.0043000000000003E-2</v>
       </c>
       <c r="CJ3" s="2" t="s">
         <v>148</v>
@@ -3387,7 +3422,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>183</v>
       </c>
@@ -3522,8 +3557,11 @@
       <c r="HU4" s="1" t="s">
         <v>394</v>
       </c>
+      <c r="IA4" s="10" t="s">
+        <v>398</v>
+      </c>
     </row>
-    <row r="5" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="S5" s="2" t="s">
         <v>210</v>
       </c>
@@ -3543,7 +3581,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>212</v>
       </c>
@@ -3662,7 +3700,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O7" s="2">
         <v>0.1</v>
       </c>
@@ -4217,8 +4255,17 @@
       <c r="HY7" s="2" t="s">
         <v>248</v>
       </c>
+      <c r="IA7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="IB7" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="IC7" s="2" t="s">
+        <v>248</v>
+      </c>
     </row>
-    <row r="8" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>265</v>
       </c>
@@ -4869,8 +4916,18 @@
         <f>EXP(-2*HU8*HX8/55.51)</f>
         <v>0.95868116900428202</v>
       </c>
+      <c r="IA8" s="2">
+        <f>(1/IB8)/P3</f>
+        <v>15.002512920914251</v>
+      </c>
+      <c r="IB8" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="IC8" s="2">
+        <v>0.73199999999999998</v>
+      </c>
     </row>
-    <row r="9" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>272</v>
       </c>
@@ -5277,7 +5334,7 @@
         <v>0.86770000000000003</v>
       </c>
       <c r="EY9">
-        <f t="shared" ref="EY9:EY18" si="62">EXP(-2*EU9*EX9/55.51)</f>
+        <f t="shared" ref="EY9:EY13" si="62">EXP(-2*EU9*EX9/55.51)</f>
         <v>0.99066499358569005</v>
       </c>
       <c r="FA9" s="2">
@@ -5320,18 +5377,18 @@
         <v>1.6080000000000001</v>
       </c>
       <c r="FN9" s="2">
-        <f t="shared" ref="FN9:FN14" si="69">$AP$3*FM9/(1+$AP$3*FM9)</f>
+        <f t="shared" ref="FN9:FN13" si="69">$AP$3*FM9/(1+$AP$3*FM9)</f>
         <v>0.16061751690516321</v>
       </c>
       <c r="FO9" s="2">
-        <f t="shared" ref="FO9:FO14" si="70">FN9*$AP$3/(FN9*$AP$3+(1-FN9)*$P$3)</f>
+        <f t="shared" ref="FO9:FO13" si="70">FN9*$AP$3/(FN9*$AP$3+(1-FN9)*$P$3)</f>
         <v>0.55830310719236997</v>
       </c>
       <c r="FP9" s="2">
         <v>0.96</v>
       </c>
       <c r="FQ9">
-        <f t="shared" ref="FQ9:FQ15" si="71">EXP(-2*FM9*FP9/55.51)</f>
+        <f t="shared" ref="FQ9:FQ13" si="71">EXP(-2*FM9*FP9/55.51)</f>
         <v>0.94590031870385338</v>
       </c>
       <c r="FS9" s="2">
@@ -5356,11 +5413,11 @@
         <v>2.2440000000000002</v>
       </c>
       <c r="FZ9" s="2">
-        <f t="shared" ref="FZ9:FZ16" si="75">$AR$3*FY9/(1+$AR$3*FY9)</f>
+        <f t="shared" ref="FZ9:FZ13" si="75">$AR$3*FY9/(1+$AR$3*FY9)</f>
         <v>0.32320195537242424</v>
       </c>
       <c r="GA9" s="2">
-        <f t="shared" ref="GA9:GA16" si="76">FZ9*$AR$3/(FZ9*$AR$3+(1-FZ9)*$P$3)</f>
+        <f t="shared" ref="GA9:GA13" si="76">FZ9*$AR$3/(FZ9*$AR$3+(1-FZ9)*$P$3)</f>
         <v>0.84942514211339359</v>
       </c>
       <c r="GB9" s="2">
@@ -5385,7 +5442,7 @@
         <v>0.82</v>
       </c>
       <c r="GI9">
-        <f t="shared" ref="GI9:GI13" si="80">EXP(-2*GE9*GH9/55.51)</f>
+        <f t="shared" ref="GI9:GI12" si="80">EXP(-2*GE9*GH9/55.51)</f>
         <v>0.95535204415515373</v>
       </c>
       <c r="GK9" s="2">
@@ -5421,7 +5478,7 @@
         <v>1.25</v>
       </c>
       <c r="GU9">
-        <f t="shared" ref="GU9:GU15" si="86">EXP(-2*GQ9*GT9/55.51)</f>
+        <f t="shared" ref="GU9:GU12" si="86">EXP(-2*GQ9*GT9/55.51)</f>
         <v>0.93619258924061399</v>
       </c>
       <c r="GW9" s="2">
@@ -5493,7 +5550,7 @@
         <v>1.27</v>
       </c>
       <c r="HS9">
-        <f t="shared" ref="HS9:HS15" si="98">EXP(-2*HO9*HR9/55.51)</f>
+        <f t="shared" ref="HS9:HS12" si="98">EXP(-2*HO9*HR9/55.51)</f>
         <v>0.96679475950506333</v>
       </c>
       <c r="HU9" s="2">
@@ -5514,8 +5571,18 @@
         <f t="shared" ref="HY9:HY15" si="101">EXP(-2*HU9*HX9/55.51)</f>
         <v>0.94720752122541474</v>
       </c>
+      <c r="IA9" s="2">
+        <f>(1/IB9)/P3</f>
+        <v>16.326264060994923</v>
+      </c>
+      <c r="IB9" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="IC9" s="2">
+        <v>0.71499999999999997</v>
+      </c>
     </row>
-    <row r="10" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O10" s="2">
         <v>3</v>
       </c>
@@ -6150,8 +6217,18 @@
         <f t="shared" si="101"/>
         <v>0.93748198497898005</v>
       </c>
+      <c r="IA10" s="2">
+        <f>(1/IB10)/P3</f>
+        <v>17.346655564807104</v>
+      </c>
+      <c r="IB10" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="IC10" s="2">
+        <v>0.70599999999999996</v>
+      </c>
     </row>
-    <row r="11" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>281</v>
       </c>
@@ -6798,8 +6875,18 @@
         <f t="shared" si="101"/>
         <v>0.92320282503628792</v>
       </c>
+      <c r="IA11" s="2">
+        <f>(1/IB10)/P3</f>
+        <v>17.346655564807104</v>
+      </c>
+      <c r="IB11" s="2">
+        <v>3</v>
+      </c>
+      <c r="IC11" s="2">
+        <v>0.69699999999999995</v>
+      </c>
     </row>
-    <row r="12" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>289</v>
       </c>
@@ -7429,8 +7516,18 @@
         <f t="shared" si="101"/>
         <v>0.91287906642256578</v>
       </c>
+      <c r="IA12" s="2">
+        <f>(1/IB11)/P3</f>
+        <v>18.503099269127578</v>
+      </c>
+      <c r="IB12" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="IC12" s="2">
+        <v>0.68600000000000005</v>
+      </c>
     </row>
-    <row r="13" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>298</v>
       </c>
@@ -8007,8 +8104,18 @@
         <f t="shared" si="101"/>
         <v>0.89510498339874134</v>
       </c>
+      <c r="IA13" s="2">
+        <f>(1/IB12)/P3</f>
+        <v>19.141137174959567</v>
+      </c>
+      <c r="IB13" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="IC13" s="2">
+        <v>0.67600000000000005</v>
+      </c>
     </row>
-    <row r="14" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>304</v>
       </c>
@@ -8480,8 +8587,18 @@
         <f t="shared" si="101"/>
         <v>0.87980202548305697</v>
       </c>
+      <c r="IA14" s="2">
+        <f>(1/IB13)/P3</f>
+        <v>19.824749216922406</v>
+      </c>
+      <c r="IB14" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="IC14" s="2">
+        <v>0.66500000000000004</v>
+      </c>
     </row>
-    <row r="15" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>311</v>
       </c>
@@ -8950,8 +9067,18 @@
         <f t="shared" si="101"/>
         <v>0.82210642126294919</v>
       </c>
+      <c r="IA15" s="2">
+        <f>(1/IB14)/P3</f>
+        <v>20.558999187919532</v>
+      </c>
+      <c r="IB15" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="IC15" s="2">
+        <v>0.65400000000000003</v>
+      </c>
     </row>
-    <row r="16" spans="1:233" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>318</v>
       </c>
@@ -9295,8 +9422,18 @@
         <v>0.96762275008731913</v>
       </c>
       <c r="EY16"/>
+      <c r="IA16" s="2">
+        <f>(1/IB15)/P3</f>
+        <v>21.349729925916435</v>
+      </c>
+      <c r="IB16" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="IC16" s="2">
+        <v>0.64500000000000002</v>
+      </c>
     </row>
-    <row r="17" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>326</v>
       </c>
@@ -9643,8 +9780,18 @@
         <v>0.96114536582444166</v>
       </c>
       <c r="EY17"/>
+      <c r="IA17" s="2">
+        <f>(1/IB16)/P3</f>
+        <v>22.203719122953096</v>
+      </c>
+      <c r="IB17" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="IC17" s="2">
+        <v>0.629</v>
+      </c>
     </row>
-    <row r="18" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="V18" s="2">
         <v>5</v>
       </c>
@@ -9965,8 +10112,18 @@
         <v>0.95464461253083843</v>
       </c>
       <c r="EY18"/>
+      <c r="IA18" s="2">
+        <f>(1/IB17)/P3</f>
+        <v>23.128874086409475</v>
+      </c>
+      <c r="IB18" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="IC18" s="2">
+        <v>0.62</v>
+      </c>
     </row>
-    <row r="19" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>338</v>
       </c>
@@ -10270,8 +10427,18 @@
         <f t="shared" si="59"/>
         <v>0.9481058402815703</v>
       </c>
+      <c r="IA19" s="2">
+        <f>(1/IB18)/P3</f>
+        <v>24.134477307557713</v>
+      </c>
+      <c r="IB19" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="IC19" s="2">
+        <v>0.51900000000000002</v>
+      </c>
     </row>
-    <row r="20" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>345</v>
       </c>
@@ -10549,8 +10716,18 @@
         <f t="shared" si="59"/>
         <v>0.94153043639048362</v>
       </c>
+      <c r="IA20" s="2">
+        <f>(1/IB19)/P3</f>
+        <v>37.006198538255155</v>
+      </c>
+      <c r="IB20" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="IC20" s="2">
+        <v>0.39200000000000002</v>
+      </c>
     </row>
-    <row r="21" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>351</v>
       </c>
@@ -10752,8 +10929,18 @@
         <f t="shared" si="59"/>
         <v>0.93492517765215333</v>
       </c>
+      <c r="IA21" s="2">
+        <f>(1/IB20)/P3</f>
+        <v>69.386622259228417</v>
+      </c>
+      <c r="IB21" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="IC21" s="2">
+        <v>0.29199999999999998</v>
+      </c>
     </row>
-    <row r="22" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>355</v>
       </c>
@@ -10956,7 +11143,7 @@
         <v>0.92157439663809559</v>
       </c>
     </row>
-    <row r="23" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>364</v>
       </c>
@@ -11145,7 +11332,7 @@
         <v>0.91147768727147049</v>
       </c>
     </row>
-    <row r="24" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>366</v>
       </c>
@@ -11249,7 +11436,19 @@
         <v>0.90126166538009622</v>
       </c>
     </row>
-    <row r="25" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2000</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>396</v>
+      </c>
       <c r="BC25" s="2">
         <v>6.9850000000000003</v>
       </c>
@@ -11327,7 +11526,7 @@
         <v>0.88750605177911046</v>
       </c>
     </row>
-    <row r="26" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="BC26" s="2">
         <v>7.4950000000000001</v>
       </c>
@@ -11391,7 +11590,7 @@
         <v>0.87710984737211428</v>
       </c>
     </row>
-    <row r="27" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="BC27" s="2">
         <v>7.9480000000000004</v>
       </c>
@@ -11455,7 +11654,7 @@
         <v>0.8667217477376794</v>
       </c>
     </row>
-    <row r="28" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="BC28" s="2">
         <v>7.9969999999999999</v>
       </c>
@@ -11519,7 +11718,7 @@
         <v>0.8490882556844872</v>
       </c>
     </row>
-    <row r="29" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="BC29" s="2">
         <v>8.9870000000000001</v>
       </c>
@@ -11583,7 +11782,7 @@
         <v>0.83139404553783947</v>
       </c>
     </row>
-    <row r="30" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="BC30" s="2">
         <v>9.9670000000000005</v>
       </c>
@@ -11647,7 +11846,7 @@
         <v>0.81356716887718761</v>
       </c>
     </row>
-    <row r="31" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="BC31" s="2">
         <v>11.013</v>
       </c>
@@ -11711,7 +11910,7 @@
         <v>0.79572679892361964</v>
       </c>
     </row>
-    <row r="32" spans="1:155" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="BC32" s="2">
         <v>11.999000000000001</v>
       </c>

</xml_diff>

<commit_message>
add kosmotrope/chaotrope analysis, update sources
</commit_message>
<xml_diff>
--- a/data/sources_list_.xlsx
+++ b/data/sources_list_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clara/Downloads/RE_ ML for AWH Discussion/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/peterbaz_stanford_edu/Documents/DiazMarin2026/hygroscopic-salts-main/hygroscopic-salts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1905FFE-40A5-1548-B975-09D0200E2583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{B1905FFE-40A5-1548-B975-09D0200E2583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{989B469D-EB29-4C37-8146-2D70258328C0}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="760" windowWidth="17860" windowHeight="17840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12730" yWindow="2770" windowWidth="25800" windowHeight="15740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sources" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="425">
   <si>
     <t xml:space="preserve">Data Source </t>
   </si>
@@ -431,21 +431,12 @@
     <t>Entropy of Mixing of Nonideal Solutions</t>
   </si>
   <si>
-    <t>Heavy math on entropy of mixing</t>
-  </si>
-  <si>
     <t>International Equations for the Saturation Properties of Ordinary Water Substance. Revised According to the International Temperature Scale of 1990. Addendum to J. Phys. Chem. Ref. Data 16, 893 (1987)</t>
   </si>
   <si>
-    <t>Reference values for pure water logic</t>
-  </si>
-  <si>
     <t>Dynamic water absorption-desorption by aqueous salt solutions</t>
   </si>
   <si>
-    <t>AD modelling and several plots for activity coefficient and uptake</t>
-  </si>
-  <si>
     <t>List of endothermic salts, NaCl, KCl, NH4OH, NH4Cl, KBr, NH4ClO3, KNO3, NaNO3</t>
   </si>
   <si>
@@ -1236,6 +1227,90 @@
   </si>
   <si>
     <t>mole ratio (water:salt)</t>
+  </si>
+  <si>
+    <t>Molecular dynamics simulations of aqueous LiCl solutions at room temperature through the entire concentration range</t>
+  </si>
+  <si>
+    <t>Provides RDFs, uses FFs</t>
+  </si>
+  <si>
+    <t>Structural, Dynamical, and Rheological Properties of KCl–Water Systems Across Varying Concentrations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provides RDFs, uses SPC/E </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference values for pure water </t>
+  </si>
+  <si>
+    <t>CDM: AD modelling and several plots for activity coefficient and uptake</t>
+  </si>
+  <si>
+    <t>Ab Initio Molecular Dynamics Simulations of the Influence of Lithium Bromide on the Structure of the Aqueous Solution–Air Interface</t>
+  </si>
+  <si>
+    <t>Provides (surface) RDFs, uses AIMD</t>
+  </si>
+  <si>
+    <t>Computer Simulation Study of the Structure of LiCl Aqueous Solutions: Test of Non-Standard Mixing Rules in the Ion Interaction</t>
+  </si>
+  <si>
+    <t>Provides RDFs, uses TIP4P-Ew</t>
+  </si>
+  <si>
+    <t>Ion–Ion Structural Correlation and Dynamics of Water in Aqueous NaCl Solutions with a Wide Range of Concentrations</t>
+  </si>
+  <si>
+    <t>System-Size Dependence of Electrolyte Activity Coefficients in Molecular Simulations</t>
+  </si>
+  <si>
+    <t>Size effects strongest at low solute concentrations, then screened</t>
+  </si>
+  <si>
+    <t>Anomalous water diffusion in salt solutions</t>
+  </si>
+  <si>
+    <t>Uses AIMD, says dynamics need quantum</t>
+  </si>
+  <si>
+    <t>Identification of Ion Pairs in Aqueous NaCl and KCl Solutions in Combination with Raman Spectroscopy, Molecular Dynamics, and Quantum Chemical Calculations</t>
+  </si>
+  <si>
+    <t>KCl forms more pairs than NaCl</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Concentration-dependent structure and dynamics of aqueous LiCl solutions: A molecular dynamics study</t>
+  </si>
+  <si>
+    <t>Accurate Simulations of Water and Aqueous Solutions through Fine-Tuned Dispersion-Corrected Density Functional Theory and Machine-Learning Interatomic Potentials</t>
+  </si>
+  <si>
+    <t>Trains and uses MLIPs, provides one for MgCl2</t>
+  </si>
+  <si>
+    <t>MLIPs</t>
+  </si>
+  <si>
+    <t>Machine learning potentials for complex aqueous systems made simple</t>
+  </si>
+  <si>
+    <t>Trains and uses MLIPs</t>
+  </si>
+  <si>
+    <t>Why Dissolving Salt in Water Decreases Its Dielectric Permittivity</t>
+  </si>
+  <si>
+    <t>Disruption of dipolar correlations among water</t>
+  </si>
+  <si>
+    <t>THERMODYNAMICS OF ELECTROLYTES. II. ACTIVITY AND OSMOTIC COEFFICIENTS FOR STRONG</t>
+  </si>
+  <si>
+    <t>Pitzer chapter</t>
   </si>
 </sst>
 </file>
@@ -2067,15 +2142,15 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="25.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="25.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="25.5" style="2" customWidth="1"/>
-    <col min="5" max="8" width="13.1640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="25.5" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="25.5" style="2"/>
+    <col min="1" max="4" width="25.453125" style="2" customWidth="1"/>
+    <col min="5" max="8" width="13.1796875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25.453125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="25.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2107,7 +2182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -2139,7 +2214,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -2168,7 +2243,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -2188,7 +2263,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -2211,7 +2286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
@@ -2225,7 +2300,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -2236,7 +2311,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
@@ -2253,7 +2328,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>46</v>
       </c>
@@ -2279,7 +2354,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="160" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="160" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>53</v>
       </c>
@@ -2308,7 +2383,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>60</v>
       </c>
@@ -2331,10 +2406,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>65</v>
       </c>
@@ -2348,7 +2423,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>68</v>
       </c>
@@ -2369,7 +2444,7 @@
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>73</v>
       </c>
@@ -2378,7 +2453,7 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>74</v>
       </c>
@@ -2386,12 +2461,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C24" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>76</v>
       </c>
@@ -2414,7 +2489,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>83</v>
       </c>
@@ -2443,10 +2518,10 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
     </row>
@@ -2474,24 +2549,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="94" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:D17"/>
+    <sheetView topLeftCell="A10" zoomScale="94" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="25.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="25.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="25.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="2" customWidth="1"/>
-    <col min="7" max="9" width="13.1640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="25.5" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="25.5" style="2"/>
+    <col min="1" max="3" width="25.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" style="2" customWidth="1"/>
+    <col min="7" max="9" width="13.1796875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.453125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="25.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -2514,7 +2589,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>95</v>
       </c>
@@ -2531,7 +2606,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>98</v>
       </c>
@@ -2548,7 +2623,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>101</v>
       </c>
@@ -2568,7 +2643,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>104</v>
       </c>
@@ -2585,7 +2660,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="320" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="320" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>107</v>
       </c>
@@ -2605,7 +2680,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>110</v>
       </c>
@@ -2622,10 +2697,10 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>113</v>
       </c>
@@ -2642,7 +2717,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>116</v>
       </c>
@@ -2665,7 +2740,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>121</v>
       </c>
@@ -2694,7 +2769,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="80" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>126</v>
       </c>
@@ -2715,6 +2790,40 @@
       </c>
       <c r="G12" s="4" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>
@@ -2734,6 +2843,8 @@
     <hyperlink ref="I11" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
     <hyperlink ref="A12" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
     <hyperlink ref="G12" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="A13" r:id="rId16" xr:uid="{35B3FE1E-225F-4F11-A434-FED1F127508A}"/>
+    <hyperlink ref="A14" r:id="rId17" location="data-availability" xr:uid="{1C0C64C2-D76C-4F34-B64D-29511E5CFC85}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2741,21 +2852,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="94" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="25.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="25.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="25.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.5" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="25.5" style="2"/>
+    <col min="1" max="2" width="25.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="25.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -2766,37 +2877,169 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="C2" s="2">
         <v>1972</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="112" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>133</v>
+        <v>401</v>
       </c>
       <c r="C3" s="2">
         <v>1992</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>402</v>
       </c>
       <c r="C4" s="2">
         <v>2024</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2023</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1973</v>
       </c>
     </row>
   </sheetData>
@@ -2804,6 +3047,17 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
     <hyperlink ref="A4" r:id="rId3" location="mmc1" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="A7" r:id="rId4" xr:uid="{08F127F5-9EA7-4FFF-BB51-B323DA2E844A}"/>
+    <hyperlink ref="A8" r:id="rId5" xr:uid="{68F40AC7-4022-400A-AE40-067AD66439A3}"/>
+    <hyperlink ref="A9" r:id="rId6" xr:uid="{A0E763A8-4A6D-4AA7-97CB-644D3FFFC184}"/>
+    <hyperlink ref="A10" r:id="rId7" display="https://pubs.acs.org/doi/10.1021/jp500937h" xr:uid="{081DD732-8280-40F7-B7E4-17777DC7D77E}"/>
+    <hyperlink ref="A11" r:id="rId8" xr:uid="{23FEF26C-03DA-4871-B3DA-C07B7A66C697}"/>
+    <hyperlink ref="A12" r:id="rId9" xr:uid="{4A838306-8DF7-4F9A-BE51-F9587D71DDCE}"/>
+    <hyperlink ref="A13" r:id="rId10" location="r42" xr:uid="{1749335F-75E3-4FA8-AAD4-5D4CE3AF6265}"/>
+    <hyperlink ref="A14" r:id="rId11" xr:uid="{78859ADF-B73D-488A-9E68-8E2538811979}"/>
+    <hyperlink ref="A6" r:id="rId12" location="f0020" xr:uid="{3D127DDF-15D8-4D0F-B660-EA132649BB31}"/>
+    <hyperlink ref="A15" r:id="rId13" xr:uid="{E7BCA44C-3428-44F3-B154-B94112E922FB}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{04B3FA29-0EB6-40C4-8E37-737739683077}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2813,250 +3067,250 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:IC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HX3" zoomScale="143" workbookViewId="0">
+    <sheetView topLeftCell="HX3" zoomScale="143" workbookViewId="0">
       <selection activeCell="IA11" sqref="IA11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="49" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.453125" defaultRowHeight="49" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="2" customWidth="1"/>
-    <col min="2" max="3" width="7.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="2" customWidth="1"/>
-    <col min="5" max="6" width="20.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.5" style="2" customWidth="1"/>
-    <col min="8" max="13" width="8.5" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.5" style="6" customWidth="1"/>
-    <col min="15" max="65" width="8.5" style="2" customWidth="1"/>
-    <col min="66" max="66" width="8.33203125" style="2" customWidth="1"/>
-    <col min="67" max="120" width="8.5" style="2" customWidth="1"/>
-    <col min="121" max="121" width="8.33203125" style="2" customWidth="1"/>
-    <col min="122" max="127" width="8.5" style="2" customWidth="1"/>
-    <col min="128" max="128" width="8.33203125" style="2" customWidth="1"/>
-    <col min="129" max="131" width="8.5" style="2" customWidth="1"/>
-    <col min="132" max="133" width="8.33203125" style="2" customWidth="1"/>
-    <col min="134" max="135" width="8.5" style="2" customWidth="1"/>
-    <col min="136" max="136" width="8.33203125" style="2" customWidth="1"/>
-    <col min="137" max="138" width="8.5" style="2" customWidth="1"/>
-    <col min="139" max="140" width="8.33203125" style="2" customWidth="1"/>
-    <col min="141" max="143" width="8.5" style="2" customWidth="1"/>
-    <col min="144" max="144" width="8.33203125" style="2" customWidth="1"/>
-    <col min="145" max="147" width="8.5" style="2" customWidth="1"/>
-    <col min="148" max="148" width="8.33203125" style="2" customWidth="1"/>
-    <col min="149" max="149" width="8.5" style="2" customWidth="1"/>
-    <col min="150" max="151" width="8.33203125" style="2" customWidth="1"/>
-    <col min="152" max="152" width="8.5" style="2" customWidth="1"/>
-    <col min="153" max="153" width="8.33203125" style="2" customWidth="1"/>
-    <col min="154" max="344" width="8.5" style="2" customWidth="1"/>
-    <col min="345" max="16384" width="20.5" style="2"/>
+    <col min="1" max="1" width="20.453125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="7.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="20.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.453125" style="2" customWidth="1"/>
+    <col min="8" max="13" width="8.453125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.453125" style="6" customWidth="1"/>
+    <col min="15" max="65" width="8.453125" style="2" customWidth="1"/>
+    <col min="66" max="66" width="8.36328125" style="2" customWidth="1"/>
+    <col min="67" max="120" width="8.453125" style="2" customWidth="1"/>
+    <col min="121" max="121" width="8.36328125" style="2" customWidth="1"/>
+    <col min="122" max="127" width="8.453125" style="2" customWidth="1"/>
+    <col min="128" max="128" width="8.36328125" style="2" customWidth="1"/>
+    <col min="129" max="131" width="8.453125" style="2" customWidth="1"/>
+    <col min="132" max="133" width="8.36328125" style="2" customWidth="1"/>
+    <col min="134" max="135" width="8.453125" style="2" customWidth="1"/>
+    <col min="136" max="136" width="8.36328125" style="2" customWidth="1"/>
+    <col min="137" max="138" width="8.453125" style="2" customWidth="1"/>
+    <col min="139" max="140" width="8.36328125" style="2" customWidth="1"/>
+    <col min="141" max="143" width="8.453125" style="2" customWidth="1"/>
+    <col min="144" max="144" width="8.36328125" style="2" customWidth="1"/>
+    <col min="145" max="147" width="8.453125" style="2" customWidth="1"/>
+    <col min="148" max="148" width="8.36328125" style="2" customWidth="1"/>
+    <col min="149" max="149" width="8.453125" style="2" customWidth="1"/>
+    <col min="150" max="151" width="8.36328125" style="2" customWidth="1"/>
+    <col min="152" max="152" width="8.453125" style="2" customWidth="1"/>
+    <col min="153" max="153" width="8.36328125" style="2" customWidth="1"/>
+    <col min="154" max="344" width="8.453125" style="2" customWidth="1"/>
+    <col min="345" max="16384" width="20.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:237" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:237" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AG1" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AH1" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AI1" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AK1" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AL1" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AM1" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="AN1" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="AO1" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="AP1" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="AQ1" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="AR1" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="AS1" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="AT1" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="AU1" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="AV1" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="AW1" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="AX1" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="AY1" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="AZ1" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="BA1" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="BC1" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="AK1" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="AL1" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="AM1" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="AN1" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="AO1" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="AP1" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="AQ1" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="AR1" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="AS1" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="AT1" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="AU1" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="AV1" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="AW1" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="AX1" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="AY1" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="AZ1" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="BA1" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="BC1" s="4" t="s">
-        <v>161</v>
-      </c>
       <c r="BD1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="BG1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BT1" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BU1" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BV1" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="BT1" s="8" t="s">
+      <c r="BW1" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="BU1" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="BV1" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="BW1" s="8" t="s">
-        <v>158</v>
-      </c>
     </row>
-    <row r="2" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>93</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -3179,75 +3433,75 @@
         <v>80.043000000000006</v>
       </c>
       <c r="BD2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BG2" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="BE2" s="2" t="s">
+      <c r="BH2" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="BF2" s="2" t="s">
+      <c r="BI2" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="BG2" s="2" t="s">
+      <c r="BJ2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="BH2" s="2" t="s">
+      <c r="BK2" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="BI2" s="2" t="s">
+      <c r="BL2" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="BJ2" s="2" t="s">
+      <c r="BM2" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="BK2" s="2" t="s">
+      <c r="BN2" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="BL2" s="2" t="s">
+      <c r="BO2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="BP2" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="BM2" s="2" t="s">
+      <c r="BQ2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="BR2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="BS2" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="BN2" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="BO2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="BP2" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="BQ2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="BR2" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="BS2" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>178</v>
-      </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C3" s="2">
         <v>2024</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -3404,303 +3658,303 @@
         <v>8.0043000000000003E-2</v>
       </c>
       <c r="CJ3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="CK3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="CM3" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="CK3" s="2" t="s">
+      <c r="CN3" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="CM3" s="2" t="s">
+      <c r="CO3" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CP3" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="CN3" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="CO3" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="CP3" s="2" t="s">
-        <v>154</v>
-      </c>
     </row>
-    <row r="4" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C4" s="2">
         <v>2007</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="P4" s="1"/>
       <c r="V4" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AK4" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AP4" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AT4" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="AP4" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="AT4" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="BA4" s="7"/>
       <c r="BB4" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="BL4" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BV4" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="CA4" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BL4" s="1" t="s">
+      <c r="CF4" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="BV4" s="1" t="s">
+      <c r="CK4" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="CA4" s="1" t="s">
+      <c r="CP4" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="CF4" s="1" t="s">
+      <c r="CU4" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="CK4" s="1" t="s">
+      <c r="CZ4" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="CP4" s="1" t="s">
+      <c r="DE4" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="CU4" s="1" t="s">
+      <c r="DJ4" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="CZ4" s="1" t="s">
+      <c r="DO4" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="DE4" s="1" t="s">
+      <c r="DT4" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="DJ4" s="1" t="s">
+      <c r="DY4" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="DO4" s="1" t="s">
+      <c r="ED4" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="DT4" s="1" t="s">
+      <c r="EI4" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="DY4" s="1" t="s">
+      <c r="EO4" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="EU4" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="FA4" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="FG4" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="FM4" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="FS4" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="FY4" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="GE4" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="GK4" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="GQ4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="GW4" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="HC4" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="HI4" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="HO4" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="HU4" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="IA4" s="10" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="5" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="S5" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="ED4" s="1" t="s">
+      <c r="T5" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="EI4" s="1" t="s">
+      <c r="Y5" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AI5" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AN5" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="EO4" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="EU4" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="FA4" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="FG4" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="FM4" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="FS4" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="FY4" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="GE4" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="GK4" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="GQ4" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="GW4" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="HC4" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="HI4" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="HO4" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="HU4" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="IA4" s="10" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="5" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="S5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="AI5" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="AN5" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="C6" s="2">
         <v>2001</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="R6" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="T6" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y6" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="AA6" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="AB6" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="T6" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="X6" s="2" t="s">
+      <c r="AC6" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD6" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="Y6" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AF6" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="AB6" s="2" t="s">
+      <c r="AG6" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="AC6" s="2" t="s">
+      <c r="AH6" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="AD6" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="AF6" s="2" t="s">
+      <c r="AI6" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AK6" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="AG6" s="2" t="s">
+      <c r="AL6" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="AH6" s="2" t="s">
+      <c r="AM6" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="AI6" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="AK6" s="2" t="s">
+      <c r="AN6" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AP6" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="AL6" s="2" t="s">
+      <c r="AQ6" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="AM6" s="2" t="s">
+      <c r="AR6" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="AN6" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="AP6" s="2" t="s">
+      <c r="AW6" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="AQ6" s="2" t="s">
+      <c r="BC6" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="BF6" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="BG6" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="BH6" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="AR6" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="AW6" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="BC6" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="BF6" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="BG6" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="BH6" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="BI6" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="BJ6" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="BO6" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O7" s="2">
         <v>0.1</v>
       </c>
@@ -3782,504 +4036,504 @@
         <v>0.99329999999999996</v>
       </c>
       <c r="AQ7" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="AR7" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="AT7" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="AU7" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="AR7" s="2" t="s">
+      <c r="AV7" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="AT7" s="2" t="s">
+      <c r="AW7" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="AX7" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="AU7" s="2" t="s">
+      <c r="AY7" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="AV7" s="2" t="s">
+      <c r="AZ7" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="AW7" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="AX7" s="2" t="s">
+      <c r="BC7" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="AY7" s="2" t="s">
+      <c r="BD7" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="AZ7" s="2" t="s">
+      <c r="BE7" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="BC7" s="2" t="s">
+      <c r="BF7" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="BD7" s="2" t="s">
+      <c r="BG7" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="BE7" s="2" t="s">
+      <c r="BH7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="BI7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="BJ7" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="BL7" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="BF7" s="2" t="s">
+      <c r="BM7" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="BG7" s="2" t="s">
+      <c r="BN7" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="BH7" s="2" t="s">
+      <c r="BO7" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="BI7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="BJ7" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="BL7" s="2" t="s">
+      <c r="BP7" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="BM7" s="2" t="s">
+      <c r="BQ7" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="BN7" s="2" t="s">
+      <c r="BR7" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="BO7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="BP7" s="2" t="s">
+      <c r="BS7" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="BQ7" s="2" t="s">
+      <c r="BT7" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="BR7" s="2" t="s">
+      <c r="BV7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="BW7" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="BS7" s="2" t="s">
+      <c r="BX7" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="BT7" s="2" t="s">
+      <c r="BY7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="CA7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="CB7" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="BV7" s="2" t="s">
+      <c r="CC7" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="CD7" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="BW7" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="BX7" s="2" t="s">
+      <c r="CF7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="CG7" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="BY7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="CA7" s="2" t="s">
+      <c r="CH7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="CI7" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="CB7" s="2" t="s">
+      <c r="CK7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="CL7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CM7" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="CC7" s="2" t="s">
+      <c r="CN7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="CP7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="CQ7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CR7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="CS7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="CU7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="CV7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="CW7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="CX7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="CZ7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="DA7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="DB7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="DC7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="DE7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="DF7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="DG7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="DH7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="DJ7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="DK7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="DL7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="DM7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="DO7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="DP7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="DQ7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="DR7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="DT7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="DU7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="DV7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="DW7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="DY7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="DZ7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="EA7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="EB7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="ED7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="EE7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="EF7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="EG7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="EI7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="EJ7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="EK7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="EL7" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="CD7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="CF7" s="2" t="s">
+      <c r="EM7" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="CG7" s="2" t="s">
+      <c r="EO7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="EP7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="EQ7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="ER7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="ES7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="EU7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="EV7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="EW7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="EX7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="EY7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="FA7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="FB7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="FC7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="FD7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="FE7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="FG7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="FH7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="FI7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="FJ7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="FK7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="FM7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="FN7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="FO7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="FP7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="FQ7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="FS7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="FT7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="FU7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="FV7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="FW7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="FY7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="FZ7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="GA7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="GB7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="GC7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="GE7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="GF7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="GG7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="GH7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="GI7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="GK7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="GL7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="GM7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="GN7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="GO7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="GQ7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="GR7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="GS7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="GT7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="GU7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="GW7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="GX7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="GY7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="GZ7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="HA7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="HC7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="HD7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="HE7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="HF7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="HG7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="HI7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="HJ7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="HK7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="HL7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="HM7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="HO7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="HP7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="HQ7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="HR7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="HS7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="HU7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="HV7" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="HW7" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="HX7" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="HY7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="IA7" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="IB7" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="IC7" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="CH7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="CI7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="CK7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="CL7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="CM7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="CN7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="CP7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="CQ7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="CR7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="CS7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="CU7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="CV7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="CW7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="CX7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="CZ7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="DA7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="DB7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="DC7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="DE7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="DF7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="DG7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="DH7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="DJ7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="DK7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="DL7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="DM7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="DO7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="DP7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="DQ7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="DR7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="DT7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="DU7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="DV7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="DW7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="DY7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="DZ7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="EA7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="EB7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="ED7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="EE7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="EF7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="EG7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="EI7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="EJ7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="EK7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="EL7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="EM7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="EO7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="EP7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="EQ7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="ER7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="ES7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="EU7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="EV7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="EW7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="EX7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="EY7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="FA7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="FB7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="FC7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="FD7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="FE7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="FG7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="FH7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="FI7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="FJ7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="FK7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="FM7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="FN7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="FO7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="FP7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="FQ7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="FS7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="FT7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="FU7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="FV7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="FW7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="FY7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="FZ7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="GA7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="GB7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="GC7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="GE7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="GF7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="GG7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="GH7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="GI7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="GK7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="GL7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="GM7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="GN7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="GO7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="GQ7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="GR7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="GS7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="GT7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="GU7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="GW7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="GX7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="GY7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="GZ7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="HA7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="HC7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="HD7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="HE7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="HF7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="HG7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="HI7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="HJ7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="HK7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="HL7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="HM7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="HO7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="HP7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="HQ7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="HR7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="HS7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="HU7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="HV7" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="HW7" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="HX7" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="HY7" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="IA7" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="IB7" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="IC7" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="8" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="C8" s="2">
         <v>2002</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="O8" s="2">
         <v>1</v>
@@ -4362,10 +4616,10 @@
         <v>0.98980000000000001</v>
       </c>
       <c r="AQ8" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="AR8" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="AT8" s="2">
         <v>1.0200000000000001E-2</v>
@@ -4388,7 +4642,7 @@
         <v>0.96589999999999998</v>
       </c>
       <c r="AZ8" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="BC8" s="2">
         <v>0.499</v>
@@ -4927,12 +5181,12 @@
         <v>0.73199999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C9" s="2">
         <v>1937</v>
@@ -5018,10 +5272,10 @@
         <v>0.98270000000000002</v>
       </c>
       <c r="AQ9" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="AR9" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="AT9" s="2">
         <v>5.0099999999999999E-2</v>
@@ -5044,7 +5298,7 @@
         <v>0.9355</v>
       </c>
       <c r="AZ9" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="BC9" s="2">
         <v>0.999</v>
@@ -5582,7 +5836,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O10" s="2">
         <v>3</v>
       </c>
@@ -5664,10 +5918,10 @@
         <v>0.96399999999999997</v>
       </c>
       <c r="AQ10" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AR10" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="AT10" s="2">
         <v>0.1003</v>
@@ -5690,7 +5944,7 @@
         <v>0.91769999999999996</v>
       </c>
       <c r="AZ10" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="BC10" s="2">
         <v>1.4990000000000001</v>
@@ -5742,10 +5996,10 @@
         <v>0.97499999999999998</v>
       </c>
       <c r="BS10" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="BT10" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="BV10" s="2">
         <v>0.3</v>
@@ -6228,18 +6482,18 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C11" s="2">
         <v>1962</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="O11" s="2">
         <v>4</v>
@@ -6322,10 +6576,10 @@
         <v>0.94399999999999995</v>
       </c>
       <c r="AQ11" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="AR11" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="AT11" s="2">
         <v>0.2001</v>
@@ -6348,7 +6602,7 @@
         <v>0.89759999999999995</v>
       </c>
       <c r="AZ11" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="BC11" s="2">
         <v>1.9970000000000001</v>
@@ -6400,10 +6654,10 @@
         <v>0.96599999999999997</v>
       </c>
       <c r="BS11" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="BT11" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="BV11" s="2">
         <v>0.4</v>
@@ -6886,18 +7140,18 @@
         <v>0.69699999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>292</v>
       </c>
       <c r="O12" s="2">
         <v>5</v>
@@ -6980,10 +7234,10 @@
         <v>0.92100000000000004</v>
       </c>
       <c r="AQ12" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="AR12" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="AT12" s="2">
         <v>0.29980000000000001</v>
@@ -7006,7 +7260,7 @@
         <v>0.88480000000000003</v>
       </c>
       <c r="AZ12" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="BC12" s="2">
         <v>2</v>
@@ -7055,10 +7309,10 @@
         <v>0.95399999999999996</v>
       </c>
       <c r="BS12" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="BT12" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="BV12" s="2">
         <v>0.5</v>
@@ -7527,15 +7781,15 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C13" s="2">
         <v>1951</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="O13" s="2">
         <v>6</v>
@@ -7618,10 +7872,10 @@
         <v>0.89700000000000002</v>
       </c>
       <c r="AQ13" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="AR13" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="AT13" s="2">
         <v>0.4002</v>
@@ -7644,7 +7898,7 @@
         <v>0.875</v>
       </c>
       <c r="AZ13" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="BC13" s="2">
         <v>2.4969999999999999</v>
@@ -7696,10 +7950,10 @@
         <v>0.93500000000000005</v>
       </c>
       <c r="BS13" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="BT13" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="BV13" s="2">
         <v>0.6</v>
@@ -8115,21 +8369,21 @@
         <v>0.67600000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C14" s="2">
         <v>2024</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="V14" s="2">
         <v>3</v>
@@ -8191,10 +8445,10 @@
         <v>0.871</v>
       </c>
       <c r="AQ14" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="AR14" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="AT14" s="2">
         <v>0.50019999999999998</v>
@@ -8217,7 +8471,7 @@
         <v>0.86719999999999997</v>
       </c>
       <c r="AZ14" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="BC14" s="2">
         <v>2.5009999999999999</v>
@@ -8269,10 +8523,10 @@
         <v>0.91900000000000004</v>
       </c>
       <c r="BS14" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="BT14" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="BV14" s="2">
         <v>0.7</v>
@@ -8598,18 +8852,18 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C15" s="2">
         <v>2014</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="V15" s="2">
         <v>3.5</v>
@@ -8671,10 +8925,10 @@
         <v>0.84199999999999997</v>
       </c>
       <c r="AQ15" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="AR15" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="AT15" s="2">
         <v>0.59989999999999999</v>
@@ -8697,7 +8951,7 @@
         <v>0.86050000000000004</v>
       </c>
       <c r="AZ15" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="BC15" s="2">
         <v>2.9940000000000002</v>
@@ -8749,10 +9003,10 @@
         <v>0.90400000000000003</v>
       </c>
       <c r="BS15" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="BT15" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="BV15" s="2">
         <v>0.8</v>
@@ -9078,15 +9332,15 @@
         <v>0.65400000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="V16" s="2">
         <v>4</v>
@@ -9148,10 +9402,10 @@
         <v>0.81100000000000005</v>
       </c>
       <c r="AQ16" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="AR16" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="AT16" s="2">
         <v>0.70020000000000004</v>
@@ -9174,7 +9428,7 @@
         <v>0.85470000000000002</v>
       </c>
       <c r="AZ16" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="BC16" s="2">
         <v>2.9990000000000001</v>
@@ -9226,10 +9480,10 @@
         <v>0.89800000000000002</v>
       </c>
       <c r="BS16" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="BT16" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="BV16" s="2">
         <v>1</v>
@@ -9433,18 +9687,18 @@
         <v>0.64500000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C17" s="2">
         <v>2025</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="V17" s="2">
         <v>4.5</v>
@@ -9506,10 +9760,10 @@
         <v>0.78</v>
       </c>
       <c r="AQ17" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="AR17" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="AT17" s="2">
         <v>0.80020000000000002</v>
@@ -9532,7 +9786,7 @@
         <v>0.84950000000000003</v>
       </c>
       <c r="AZ17" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="BC17" s="2">
         <v>3.496</v>
@@ -9584,10 +9838,10 @@
         <v>0.89700000000000002</v>
       </c>
       <c r="BS17" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="BT17" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="BV17" s="2">
         <v>1.5</v>
@@ -9791,7 +10045,7 @@
         <v>0.629</v>
       </c>
     </row>
-    <row r="18" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="V18" s="2">
         <v>5</v>
       </c>
@@ -9838,10 +10092,10 @@
         <v>0.748</v>
       </c>
       <c r="AQ18" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="AR18" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="AT18" s="2">
         <v>0.90010000000000001</v>
@@ -9864,7 +10118,7 @@
         <v>0.8448</v>
       </c>
       <c r="AZ18" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="BC18" s="2">
         <v>3.9950000000000001</v>
@@ -9916,10 +10170,10 @@
         <v>0.89900000000000002</v>
       </c>
       <c r="BS18" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="BT18" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="BV18" s="2">
         <v>2</v>
@@ -10123,21 +10377,21 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="19" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C19" s="2">
         <v>2022</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="V19" s="2">
         <v>5.5</v>
@@ -10185,7 +10439,7 @@
         <v>0.71399999999999997</v>
       </c>
       <c r="AR19" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="AT19" s="2">
         <v>1.002</v>
@@ -10208,7 +10462,7 @@
         <v>0.84040000000000004</v>
       </c>
       <c r="AZ19" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="BC19" s="2">
         <v>4.4969999999999999</v>
@@ -10260,10 +10514,10 @@
         <v>0.90200000000000002</v>
       </c>
       <c r="BS19" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="BT19" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="BV19" s="2">
         <v>2.5</v>
@@ -10438,18 +10692,18 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C20" s="2">
         <v>2003</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="V20" s="2">
         <v>6</v>
@@ -10497,7 +10751,7 @@
         <v>0.68</v>
       </c>
       <c r="AR20" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="BC20" s="2">
         <v>4.9859999999999998</v>
@@ -10549,10 +10803,10 @@
         <v>0.90700000000000003</v>
       </c>
       <c r="BS20" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="BT20" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="BV20" s="2">
         <v>3</v>
@@ -10727,18 +10981,18 @@
         <v>0.39200000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C21" s="2">
         <v>2003</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="BC21" s="2">
         <v>4.9909999999999997</v>
@@ -10790,10 +11044,10 @@
         <v>0.91400000000000003</v>
       </c>
       <c r="BS21" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="BT21" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="CF21" s="2">
         <v>3.5</v>
@@ -10940,18 +11194,18 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C22" s="2">
         <v>1947</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="BC22" s="2">
         <v>5.4969999999999999</v>
@@ -11003,10 +11257,10 @@
         <v>0.92100000000000004</v>
       </c>
       <c r="BS22" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="BT22" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="CF22" s="2">
         <v>4</v>
@@ -11143,18 +11397,18 @@
         <v>0.92157439663809559</v>
       </c>
     </row>
-    <row r="23" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C23" s="2">
         <v>1944</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="BC23" s="2">
         <v>6.0090000000000003</v>
@@ -11206,10 +11460,10 @@
         <v>0.92800000000000005</v>
       </c>
       <c r="BS23" s="2" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="BT23" s="2" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="CF23" s="2">
         <v>4.5</v>
@@ -11332,18 +11586,18 @@
         <v>0.91147768727147049</v>
       </c>
     </row>
-    <row r="24" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B24" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C24" s="2">
         <v>1991</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="BC24" s="2">
         <v>6.5</v>
@@ -11436,18 +11690,18 @@
         <v>0.90126166538009622</v>
       </c>
     </row>
-    <row r="25" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C25" s="2">
         <v>2000</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="BC25" s="2">
         <v>6.9850000000000003</v>
@@ -11526,7 +11780,7 @@
         <v>0.88750605177911046</v>
       </c>
     </row>
-    <row r="26" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="BC26" s="2">
         <v>7.4950000000000001</v>
       </c>
@@ -11590,7 +11844,7 @@
         <v>0.87710984737211428</v>
       </c>
     </row>
-    <row r="27" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="BC27" s="2">
         <v>7.9480000000000004</v>
       </c>
@@ -11654,7 +11908,7 @@
         <v>0.8667217477376794</v>
       </c>
     </row>
-    <row r="28" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="BC28" s="2">
         <v>7.9969999999999999</v>
       </c>
@@ -11718,7 +11972,7 @@
         <v>0.8490882556844872</v>
       </c>
     </row>
-    <row r="29" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="BC29" s="2">
         <v>8.9870000000000001</v>
       </c>
@@ -11782,7 +12036,7 @@
         <v>0.83139404553783947</v>
       </c>
     </row>
-    <row r="30" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="BC30" s="2">
         <v>9.9670000000000005</v>
       </c>
@@ -11846,7 +12100,7 @@
         <v>0.81356716887718761</v>
       </c>
     </row>
-    <row r="31" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="BC31" s="2">
         <v>11.013</v>
       </c>
@@ -11910,7 +12164,7 @@
         <v>0.79572679892361964</v>
       </c>
     </row>
-    <row r="32" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:237" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="BC32" s="2">
         <v>11.999000000000001</v>
       </c>
@@ -11974,8 +12228,8 @@
         <v>0.77752510639851602</v>
       </c>
     </row>
-    <row r="33" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="34" ht="14.5" x14ac:dyDescent="0.35"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O1" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>

</xml_diff>

<commit_message>
adjust plots for new limits
</commit_message>
<xml_diff>
--- a/data/sources_list_.xlsx
+++ b/data/sources_list_.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/peterbaz_stanford_edu/Documents/DiazMarin2026/hygroscopic-salts-main/hygroscopic-salts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="323" documentId="13_ncr:1_{B1905FFE-40A5-1548-B975-09D0200E2583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B8488F8-69F1-4E50-86A1-3151FD60EB0F}"/>
+  <xr:revisionPtr revIDLastSave="324" documentId="13_ncr:1_{B1905FFE-40A5-1548-B975-09D0200E2583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C77F5915-02D9-49E9-ACDB-8363D46C9911}"/>
   <bookViews>
     <workbookView xWindow="14160" yWindow="480" windowWidth="19560" windowHeight="19485" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3056,8 +3056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:GS34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CI9" zoomScale="75" zoomScaleNormal="32" workbookViewId="0">
-      <selection activeCell="CU25" sqref="CU25"/>
+    <sheetView tabSelected="1" topLeftCell="BG1" zoomScale="75" zoomScaleNormal="32" workbookViewId="0">
+      <selection activeCell="BL4" sqref="BL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4590,7 +4590,7 @@
         <v>0.2</v>
       </c>
       <c r="CR8" s="2">
-        <f t="shared" ref="CR8:CR18" si="18">$BW$3*CQ8/(1+$BW$3*CQ8)</f>
+        <f>$BW$3*CQ8/(1+$BW$3*CQ8)</f>
         <v>3.0934245671270493E-2</v>
       </c>
       <c r="CS8" s="2">
@@ -4600,7 +4600,7 @@
         <v>0.2</v>
       </c>
       <c r="CV8" s="2">
-        <f t="shared" ref="CV8:CV23" si="19">$BX$3*CU8/(1+$BX$3*CU8)</f>
+        <f t="shared" ref="CV8:CV23" si="18">$BX$3*CU8/(1+$BX$3*CU8)</f>
         <v>3.1278580914568345E-2</v>
       </c>
       <c r="CW8" s="2">
@@ -4610,7 +4610,7 @@
         <v>0.1</v>
       </c>
       <c r="CZ8" s="2">
-        <f t="shared" ref="CZ8:CZ20" si="20">$BY$3*CY8/(1+$BY$3*CY8)</f>
+        <f t="shared" ref="CZ8:CZ20" si="19">$BY$3*CY8/(1+$BY$3*CY8)</f>
         <v>6.8487708760388358E-3</v>
       </c>
       <c r="DA8" s="2">
@@ -4620,7 +4620,7 @@
         <v>0.1</v>
       </c>
       <c r="DD8" s="2">
-        <f t="shared" ref="DD8:DD18" si="21">$BZ$3*DC8/(1+$BZ$3*DC8)</f>
+        <f t="shared" ref="DD8:DD18" si="20">$BZ$3*DC8/(1+$BZ$3*DC8)</f>
         <v>1.0008810921582798E-2</v>
       </c>
       <c r="DE8" s="2">
@@ -4640,7 +4640,7 @@
         <v>0.1</v>
       </c>
       <c r="DL8" s="2">
-        <f t="shared" ref="DL8:DL23" si="22">$CB$3*DK8/(1+$CB$3*DK8)</f>
+        <f t="shared" ref="DL8:DL23" si="21">$CB$3*DK8/(1+$CB$3*DK8)</f>
         <v>1.6145059572416642E-2</v>
       </c>
       <c r="DM8" s="2">
@@ -4657,7 +4657,7 @@
         <v>0.91900000000000004</v>
       </c>
       <c r="DR8">
-        <f t="shared" ref="DR8:DR32" si="23">EXP(-2*DO8*DQ8/55.51)</f>
+        <f t="shared" ref="DR8:DR32" si="22">EXP(-2*DO8*DQ8/55.51)</f>
         <v>0.9933996484160329</v>
       </c>
       <c r="DS8"/>
@@ -4665,98 +4665,98 @@
         <v>0.2</v>
       </c>
       <c r="DU8" s="2">
-        <f t="shared" ref="DU8:DU32" si="24">$CD$3*DT8/(1+$CD$3*DT8)</f>
+        <f t="shared" ref="DU8:DU32" si="23">$CD$3*DT8/(1+$CD$3*DT8)</f>
         <v>2.3902671383168955E-2</v>
       </c>
       <c r="DV8" s="2">
         <v>0.95750000000000002</v>
       </c>
       <c r="DW8">
-        <f t="shared" ref="DW8:DW32" si="25">EXP(-2*DT8*DV8/55.51)</f>
+        <f t="shared" ref="DW8:DW32" si="24">EXP(-2*DT8*DV8/55.51)</f>
         <v>0.99312409026993709</v>
       </c>
       <c r="DY8" s="2">
         <v>0.2</v>
       </c>
       <c r="DZ8" s="2">
-        <f t="shared" ref="DZ8:DZ13" si="26">$CE$3*DY8/(1+$CE$3*DY8)</f>
+        <f t="shared" ref="DZ8:DZ13" si="25">$CE$3*DY8/(1+$CE$3*DY8)</f>
         <v>2.3923631784950855E-2</v>
       </c>
       <c r="EA8" s="2">
         <v>0.88759999999999994</v>
       </c>
       <c r="EB8">
-        <f t="shared" ref="EB8:EB13" si="27">EXP(-2*DY8*EA8/55.51)</f>
+        <f t="shared" ref="EB8:EB13" si="26">EXP(-2*DY8*EA8/55.51)</f>
         <v>0.99362444595268207</v>
       </c>
       <c r="ED8" s="2">
         <v>2.0030000000000001</v>
       </c>
       <c r="EE8" s="2">
-        <f t="shared" ref="EE8:EE13" si="28">$CF$3*ED8/(1+$CF$3*ED8)</f>
+        <f t="shared" ref="EE8:EE13" si="27">$CF$3*ED8/(1+$CF$3*ED8)</f>
         <v>0.17087356437897722</v>
       </c>
       <c r="EF8" s="2">
         <v>1.02</v>
       </c>
       <c r="EG8">
-        <f t="shared" ref="EG8:EG13" si="29">EXP(-2*ED8*EF8/55.51)</f>
+        <f t="shared" ref="EG8:EG13" si="28">EXP(-2*ED8*EF8/55.51)</f>
         <v>0.92903346275659915</v>
       </c>
       <c r="EI8" s="2">
         <v>1.004</v>
       </c>
       <c r="EJ8" s="2">
-        <f t="shared" ref="EJ8:EJ15" si="30">$CG$3*EI8/(1+$CG$3*EI8)</f>
+        <f t="shared" ref="EJ8:EJ15" si="29">$CG$3*EI8/(1+$CG$3*EI8)</f>
         <v>0.13080480278326037</v>
       </c>
       <c r="EK8" s="2">
         <v>0.93</v>
       </c>
       <c r="EL8">
-        <f t="shared" ref="EL8:EL15" si="31">EXP(-2*EI8*EK8/55.51)</f>
+        <f t="shared" ref="EL8:EL15" si="30">EXP(-2*EI8*EK8/55.51)</f>
         <v>0.96691807680701369</v>
       </c>
       <c r="EN8" s="2">
         <v>1.2549999999999999</v>
       </c>
       <c r="EO8" s="2">
-        <f t="shared" ref="EO8:EO13" si="32">$CH$3*EN8/(1+$CH$3*EN8)</f>
+        <f t="shared" ref="EO8:EO13" si="31">$CH$3*EN8/(1+$CH$3*EN8)</f>
         <v>0.12993922625495388</v>
       </c>
       <c r="EP8" s="2">
         <v>1.07</v>
       </c>
       <c r="EQ8">
-        <f t="shared" ref="EQ8:EQ13" si="33">EXP(-2*EN8*EP8/55.51)</f>
+        <f t="shared" ref="EQ8:EQ13" si="32">EXP(-2*EN8*EP8/55.51)</f>
         <v>0.95276949895611107</v>
       </c>
       <c r="ES8" s="2">
         <v>1.4930000000000001</v>
       </c>
       <c r="ET8" s="2">
-        <f t="shared" ref="ET8:ET13" si="34">$CI$3*ES8/(1+$CI$3*ES8)</f>
+        <f t="shared" ref="ET8:ET13" si="33">$CI$3*ES8/(1+$CI$3*ES8)</f>
         <v>0.15292539417515585</v>
       </c>
       <c r="EU8" s="2">
         <v>0.9</v>
       </c>
       <c r="EV8">
-        <f t="shared" ref="EV8:EV13" si="35">EXP(-2*ES8*EU8/55.51)</f>
+        <f t="shared" ref="EV8:EV13" si="34">EXP(-2*ES8*EU8/55.51)</f>
         <v>0.95274032072972648</v>
       </c>
       <c r="EX8" s="2">
         <v>1.57</v>
       </c>
       <c r="EY8" s="2">
-        <f t="shared" ref="EY8:EY13" si="36">$CJ$3*EX8/(1+$CJ$3*EX8)</f>
+        <f t="shared" ref="EY8:EY13" si="35">$CJ$3*EX8/(1+$CJ$3*EX8)</f>
         <v>0.25043757580418491</v>
       </c>
       <c r="EZ8" s="2">
         <v>0.94</v>
       </c>
       <c r="FA8">
-        <f t="shared" ref="FA8:FA13" si="37">EXP(-2*EX8*EZ8/55.51)</f>
+        <f t="shared" ref="FA8:FA13" si="36">EXP(-2*EX8*EZ8/55.51)</f>
         <v>0.9482165245628732</v>
       </c>
       <c r="FC8" s="2">
@@ -4777,14 +4777,14 @@
         <v>1.006</v>
       </c>
       <c r="FI8" s="2">
-        <f t="shared" ref="FI8:FI15" si="38">$CL$3*FH8/(1+$CL$3*FH8)</f>
+        <f t="shared" ref="FI8:FI15" si="37">$CL$3*FH8/(1+$CL$3*FH8)</f>
         <v>0.16742246667512675</v>
       </c>
       <c r="FJ8" s="2">
         <v>1.3</v>
       </c>
       <c r="FK8">
-        <f t="shared" ref="FK8:FK15" si="39">EXP(-2*FH8*FJ8/55.51)</f>
+        <f t="shared" ref="FK8:FK15" si="38">EXP(-2*FH8*FJ8/55.51)</f>
         <v>0.95397345016283042</v>
       </c>
       <c r="FM8" s="2">
@@ -4805,42 +4805,42 @@
         <v>0.66200000000000003</v>
       </c>
       <c r="FS8" s="2">
-        <f t="shared" ref="FS8:FS15" si="40">$CN$3*FR8/(1+$CN$3*FR8)</f>
+        <f t="shared" ref="FS8:FS15" si="39">$CN$3*FR8/(1+$CN$3*FR8)</f>
         <v>9.4979101528918766E-2</v>
       </c>
       <c r="FT8" s="2">
         <v>0.94</v>
       </c>
       <c r="FU8">
-        <f t="shared" ref="FU8:FU15" si="41">EXP(-2*FR8*FT8/55.51)</f>
+        <f t="shared" ref="FU8:FU15" si="40">EXP(-2*FR8*FT8/55.51)</f>
         <v>0.97782900594463251</v>
       </c>
       <c r="FW8" s="2">
         <v>0.8</v>
       </c>
       <c r="FX8" s="2">
-        <f t="shared" ref="FX8:FX15" si="42">$CO$3*FW8/(1+$CO$3*FW8)</f>
+        <f t="shared" ref="FX8:FX15" si="41">$CO$3*FW8/(1+$CO$3*FW8)</f>
         <v>0.16523643843117874</v>
       </c>
       <c r="FY8" s="2">
         <v>1.52</v>
       </c>
       <c r="FZ8">
-        <f t="shared" ref="FZ8:FZ15" si="43">EXP(-2*FW8*FY8/55.51)</f>
+        <f t="shared" ref="FZ8:FZ15" si="42">EXP(-2*FW8*FY8/55.51)</f>
         <v>0.95713395276870528</v>
       </c>
       <c r="GB8" s="2">
         <v>0.97</v>
       </c>
       <c r="GC8" s="2">
-        <f t="shared" ref="GC8:GC15" si="44">$CP$3*GB8/(1+$CP$3*GB8)</f>
+        <f t="shared" ref="GC8:GC15" si="43">$CP$3*GB8/(1+$CP$3*GB8)</f>
         <v>0.24879079732668685</v>
       </c>
       <c r="GD8" s="2">
         <v>1.26</v>
       </c>
       <c r="GE8">
-        <f t="shared" ref="GE8:GE15" si="45">EXP(-2*GB8*GD8/55.51)</f>
+        <f t="shared" ref="GE8:GE15" si="44">EXP(-2*GB8*GD8/55.51)</f>
         <v>0.95692016902693289</v>
       </c>
       <c r="GG8" s="2">
@@ -4861,14 +4861,14 @@
         <v>1.0009999999999999</v>
       </c>
       <c r="GM8" s="2">
-        <f t="shared" ref="GM8:GM15" si="46">$CR$3*GL8/(1+$CR$3*GL8)</f>
+        <f t="shared" ref="GM8:GM15" si="45">$CR$3*GL8/(1+$CR$3*GL8)</f>
         <v>0.22924975001101011</v>
       </c>
       <c r="GN8" s="2">
         <v>1.17</v>
       </c>
       <c r="GO8">
-        <f t="shared" ref="GO8:GO15" si="47">EXP(-2*GL8*GN8/55.51)</f>
+        <f t="shared" ref="GO8:GO15" si="46">EXP(-2*GL8*GN8/55.51)</f>
         <v>0.95868116900428202</v>
       </c>
       <c r="GQ8" s="2">
@@ -5102,7 +5102,7 @@
         <v>0.3</v>
       </c>
       <c r="CR9" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="CR8:CR18" si="47">$BW$3*CQ9/(1+$BW$3*CQ9)</f>
         <v>4.5694604446998244E-2</v>
       </c>
       <c r="CS9" s="2">
@@ -5112,7 +5112,7 @@
         <v>0.3</v>
       </c>
       <c r="CV9" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>4.6195407968835159E-2</v>
       </c>
       <c r="CW9" s="2">
@@ -5122,7 +5122,7 @@
         <v>0.2</v>
       </c>
       <c r="CZ9" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>1.3604368548972569E-2</v>
       </c>
       <c r="DA9" s="2">
@@ -5132,7 +5132,7 @@
         <v>0.2</v>
       </c>
       <c r="DD9" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>1.9819254670561254E-2</v>
       </c>
       <c r="DE9" s="2">
@@ -5152,7 +5152,7 @@
         <v>0.2</v>
       </c>
       <c r="DL9" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>3.1777076354059755E-2</v>
       </c>
       <c r="DM9" s="2">
@@ -5169,105 +5169,105 @@
         <v>0.91420000000000001</v>
       </c>
       <c r="DR9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.99016719844072409</v>
       </c>
       <c r="DT9" s="2">
         <v>0.3</v>
       </c>
       <c r="DU9" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>3.5430564504616423E-2</v>
       </c>
       <c r="DV9" s="2">
         <v>0.97099999999999997</v>
       </c>
       <c r="DW9">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.98955947836302427</v>
       </c>
       <c r="DY9" s="2">
         <v>0.3</v>
       </c>
       <c r="DZ9" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>3.5461266535810915E-2</v>
       </c>
       <c r="EA9" s="2">
         <v>0.86770000000000003</v>
       </c>
       <c r="EB9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0.99066499358569005</v>
       </c>
       <c r="ED9" s="2">
         <v>2.9940000000000002</v>
       </c>
       <c r="EE9" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>0.23550478464681998</v>
       </c>
       <c r="EF9" s="2">
         <v>1.19</v>
       </c>
       <c r="EG9">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.87952945746590139</v>
       </c>
       <c r="EI9" s="2">
         <v>1.673</v>
       </c>
       <c r="EJ9" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.20048992058842152</v>
       </c>
       <c r="EK9" s="2">
         <v>1.01</v>
       </c>
       <c r="EL9">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0.94093595549059772</v>
       </c>
       <c r="EN9" s="2">
         <v>1.6080000000000001</v>
       </c>
       <c r="EO9" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0.16061751690516321</v>
       </c>
       <c r="EP9" s="2">
         <v>0.96</v>
       </c>
       <c r="EQ9">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.94590031870385338</v>
       </c>
       <c r="ES9" s="2">
         <v>2.968</v>
       </c>
       <c r="ET9" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>0.26410556564614002</v>
       </c>
       <c r="EU9" s="2">
         <v>0.95</v>
       </c>
       <c r="EV9">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.90340086081526783</v>
       </c>
       <c r="EX9" s="2">
         <v>2.2440000000000002</v>
       </c>
       <c r="EY9" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.32320195537242424</v>
       </c>
       <c r="EZ9" s="2">
         <v>0.88</v>
       </c>
       <c r="FA9">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.93132380235784307</v>
       </c>
       <c r="FC9" s="2">
@@ -5288,14 +5288,14 @@
         <v>1.238</v>
       </c>
       <c r="FI9" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.19837354481350811</v>
       </c>
       <c r="FJ9" s="2">
         <v>1.37</v>
       </c>
       <c r="FK9">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>0.94072138350529388</v>
       </c>
       <c r="FM9" s="2">
@@ -5316,42 +5316,42 @@
         <v>0.871</v>
       </c>
       <c r="FS9" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>0.12132686181194545</v>
       </c>
       <c r="FT9" s="2">
         <v>0.82</v>
       </c>
       <c r="FU9">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>0.97459525126863267</v>
       </c>
       <c r="FW9" s="2">
         <v>1.0129999999999999</v>
       </c>
       <c r="FX9" s="2">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>0.20041360365441047</v>
       </c>
       <c r="FY9" s="2">
         <v>1.29</v>
       </c>
       <c r="FZ9">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0.95400885318520878</v>
       </c>
       <c r="GB9" s="2">
         <v>1.264</v>
       </c>
       <c r="GC9" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.3014650122824804</v>
       </c>
       <c r="GD9" s="2">
         <v>1.37</v>
       </c>
       <c r="GE9">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0.93951486205196444</v>
       </c>
       <c r="GG9" s="2">
@@ -5372,14 +5372,14 @@
         <v>1.2649999999999999</v>
       </c>
       <c r="GM9" s="2">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0.27319353889406656</v>
       </c>
       <c r="GN9" s="2">
         <v>1.19</v>
       </c>
       <c r="GO9">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0.94720752122541474</v>
       </c>
       <c r="GQ9" s="2">
@@ -5604,7 +5604,7 @@
         <v>0.4</v>
       </c>
       <c r="CR10" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="47"/>
         <v>6.001206342918277E-2</v>
       </c>
       <c r="CS10" s="2">
@@ -5614,7 +5614,7 @@
         <v>0.4</v>
       </c>
       <c r="CV10" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>6.0659809082487817E-2</v>
       </c>
       <c r="CW10" s="2">
@@ -5624,7 +5624,7 @@
         <v>0.3</v>
       </c>
       <c r="CZ10" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.0268681516780834E-2</v>
       </c>
       <c r="DA10" s="2">
@@ -5634,7 +5634,7 @@
         <v>0.3</v>
       </c>
       <c r="DD10" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>2.9437170615239774E-2</v>
       </c>
       <c r="DE10" s="2">
@@ -5654,7 +5654,7 @@
         <v>0.3</v>
       </c>
       <c r="DL10" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>4.6920122375456279E-2</v>
       </c>
       <c r="DM10" s="2">
@@ -5671,105 +5671,105 @@
         <v>0.91149999999999998</v>
       </c>
       <c r="DR10">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.98694953373358874</v>
       </c>
       <c r="DT10" s="2">
         <v>0.4</v>
       </c>
       <c r="DU10" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>4.668934274950047E-2</v>
       </c>
       <c r="DV10" s="2">
         <v>0.98550000000000004</v>
       </c>
       <c r="DW10">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.98589753827697413</v>
       </c>
       <c r="DY10" s="2">
         <v>0.4</v>
       </c>
       <c r="DZ10" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>4.6729328325484737E-2</v>
       </c>
       <c r="EA10" s="2">
         <v>0.84989999999999999</v>
       </c>
       <c r="EB10">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0.98782610495573842</v>
       </c>
       <c r="ED10" s="2">
         <v>4.0119999999999996</v>
       </c>
       <c r="EE10" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>0.29218306512875597</v>
       </c>
       <c r="EF10" s="2">
         <v>1.23</v>
       </c>
       <c r="EG10">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.83711221141098335</v>
       </c>
       <c r="EI10" s="2">
         <v>2.1579999999999999</v>
       </c>
       <c r="EJ10" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.24440631349300973</v>
       </c>
       <c r="EK10" s="2">
         <v>1.1100000000000001</v>
       </c>
       <c r="EL10">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0.91731491250019648</v>
       </c>
       <c r="EN10" s="2">
         <v>2.2200000000000002</v>
       </c>
       <c r="EO10" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0.20897340568589917</v>
       </c>
       <c r="EP10" s="2">
         <v>0.95</v>
       </c>
       <c r="EQ10">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.92682889589713979</v>
       </c>
       <c r="ES10" s="2">
         <v>3.55</v>
       </c>
       <c r="ET10" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>0.30034017460710605</v>
       </c>
       <c r="EU10" s="2">
         <v>0.98</v>
       </c>
       <c r="EV10">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.88219091951636441</v>
       </c>
       <c r="EX10" s="2">
         <v>2.7679999999999998</v>
       </c>
       <c r="EY10" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.37069638134309096</v>
       </c>
       <c r="EZ10" s="2">
         <v>0.81</v>
       </c>
       <c r="FA10">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.92239556281327817</v>
       </c>
       <c r="FC10" s="2">
@@ -5790,14 +5790,14 @@
         <v>1.7090000000000001</v>
       </c>
       <c r="FI10" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.25462802021278863</v>
       </c>
       <c r="FJ10" s="2">
         <v>1.47</v>
       </c>
       <c r="FK10">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>0.91346108689128158</v>
       </c>
       <c r="FM10" s="2">
@@ -5818,42 +5818,42 @@
         <v>1.2989999999999999</v>
       </c>
       <c r="FS10" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>0.17076479541975584</v>
       </c>
       <c r="FT10" s="2">
         <v>1.1200000000000001</v>
       </c>
       <c r="FU10">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>0.94893150087008038</v>
       </c>
       <c r="FW10" s="2">
         <v>1.345</v>
       </c>
       <c r="FX10" s="2">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>0.24969613631400547</v>
       </c>
       <c r="FY10" s="2">
         <v>1.22</v>
       </c>
       <c r="FZ10">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0.94259282247862319</v>
       </c>
       <c r="GB10" s="2">
         <v>1.534</v>
       </c>
       <c r="GC10" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.34372592335498442</v>
       </c>
       <c r="GD10" s="2">
         <v>1.42</v>
       </c>
       <c r="GE10">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0.92451829840074184</v>
       </c>
       <c r="GG10" s="2">
@@ -5874,14 +5874,14 @@
         <v>1.4450000000000001</v>
       </c>
       <c r="GM10" s="2">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0.30038975986088384</v>
       </c>
       <c r="GN10" s="2">
         <v>1.24</v>
       </c>
       <c r="GO10">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0.93748198497898005</v>
       </c>
       <c r="GQ10" s="2">
@@ -6118,7 +6118,7 @@
         <v>0.5</v>
       </c>
       <c r="CR11" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="47"/>
         <v>7.3906262458854816E-2</v>
       </c>
       <c r="CS11" s="2">
@@ -6128,7 +6128,7 @@
         <v>0.5</v>
       </c>
       <c r="CV11" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>7.4692059830781532E-2</v>
       </c>
       <c r="CW11" s="2">
@@ -6138,7 +6138,7 @@
         <v>0.4</v>
       </c>
       <c r="CZ11" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.6843547583457892E-2</v>
       </c>
       <c r="DA11" s="2">
@@ -6148,7 +6148,7 @@
         <v>0.4</v>
       </c>
       <c r="DD11" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>3.8868171158356085E-2</v>
       </c>
       <c r="DE11" s="2">
@@ -6168,7 +6168,7 @@
         <v>0.4</v>
       </c>
       <c r="DL11" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>6.1596786907398379E-2</v>
       </c>
       <c r="DM11" s="2">
@@ -6185,105 +6185,105 @@
         <v>0.91020000000000001</v>
       </c>
       <c r="DR11">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.98373665421648882</v>
       </c>
       <c r="DT11" s="2">
         <v>0.5</v>
       </c>
       <c r="DU11" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5.7688320989050329E-2</v>
       </c>
       <c r="DV11" s="2">
         <v>0.99950000000000006</v>
       </c>
       <c r="DW11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.98215537048432389</v>
       </c>
       <c r="DY11" s="2">
         <v>0.5</v>
       </c>
       <c r="DZ11" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>5.7737155779604719E-2</v>
       </c>
       <c r="EA11" s="2">
         <v>0.83330000000000004</v>
       </c>
       <c r="EB11">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0.98510040440198543</v>
       </c>
       <c r="ED11" s="2">
         <v>4.9889999999999999</v>
       </c>
       <c r="EE11" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>0.33920044482911493</v>
       </c>
       <c r="EF11" s="2">
         <v>1.26</v>
       </c>
       <c r="EG11">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.79732989957467659</v>
       </c>
       <c r="EI11" s="2">
         <v>3.3029999999999999</v>
       </c>
       <c r="EJ11" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.33114245477153503</v>
       </c>
       <c r="EK11" s="2">
         <v>1.26</v>
       </c>
       <c r="EL11">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0.86075356367894651</v>
       </c>
       <c r="EN11" s="2">
         <v>3.0209999999999999</v>
       </c>
       <c r="EO11" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0.26443491315550799</v>
       </c>
       <c r="EP11" s="2">
         <v>0.96</v>
       </c>
       <c r="EQ11">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.90078250538489457</v>
       </c>
       <c r="ES11" s="2">
         <v>4.4630000000000001</v>
       </c>
       <c r="ET11" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>0.35050847003203212</v>
       </c>
       <c r="EU11" s="2">
         <v>0.98</v>
       </c>
       <c r="EV11">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.85420517801429519</v>
       </c>
       <c r="EX11" s="2">
         <v>3.4849999999999999</v>
       </c>
       <c r="EY11" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.42582946899819329</v>
       </c>
       <c r="EZ11" s="2">
         <v>0.81</v>
       </c>
       <c r="FA11">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.90329508236438283</v>
       </c>
       <c r="FC11" s="2">
@@ -6304,14 +6304,14 @@
         <v>2.254</v>
       </c>
       <c r="FI11" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.31060730078174514</v>
       </c>
       <c r="FJ11" s="2">
         <v>1.71</v>
       </c>
       <c r="FK11">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>0.87034106667801636</v>
       </c>
       <c r="FM11" s="2">
@@ -6332,42 +6332,42 @@
         <v>1.5029999999999999</v>
       </c>
       <c r="FS11" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>0.192422069880542</v>
       </c>
       <c r="FT11" s="2">
         <v>1.31</v>
       </c>
       <c r="FU11">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>0.93151810707080429</v>
       </c>
       <c r="FW11" s="2">
         <v>1.746</v>
       </c>
       <c r="FX11" s="2">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>0.3016822098473172</v>
       </c>
       <c r="FY11" s="2">
         <v>1.36</v>
       </c>
       <c r="FZ11">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0.91800328077604243</v>
       </c>
       <c r="GB11" s="2">
         <v>1.96</v>
       </c>
       <c r="GC11" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.40091162080485371</v>
       </c>
       <c r="GD11" s="2">
         <v>1.6</v>
       </c>
       <c r="GE11">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0.89316079681406857</v>
       </c>
       <c r="GG11" s="2">
@@ -6388,14 +6388,14 @@
         <v>1.706</v>
       </c>
       <c r="GM11" s="2">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0.33639513539410604</v>
       </c>
       <c r="GN11" s="2">
         <v>1.3</v>
       </c>
       <c r="GO11">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0.92320282503628792</v>
       </c>
       <c r="GQ11" s="2">
@@ -6629,7 +6629,7 @@
         <v>0.6</v>
       </c>
       <c r="CR12" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="47"/>
         <v>8.7395697085313417E-2</v>
       </c>
       <c r="CS12" s="2">
@@ -6639,7 +6639,7 @@
         <v>0.6</v>
       </c>
       <c r="CV12" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>8.8311242081481708E-2</v>
       </c>
       <c r="CW12" s="2">
@@ -6649,7 +6649,7 @@
         <v>0.5</v>
       </c>
       <c r="CZ12" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>3.3330755548681458E-2</v>
       </c>
       <c r="DA12" s="2">
@@ -6659,7 +6659,7 @@
         <v>0.5</v>
       </c>
       <c r="DD12" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>4.8117652658131449E-2</v>
       </c>
       <c r="DE12" s="2">
@@ -6669,7 +6669,7 @@
         <v>0.5</v>
       </c>
       <c r="DL12" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>7.5828288896076887E-2</v>
       </c>
       <c r="DM12" s="2">
@@ -6686,105 +6686,105 @@
         <v>0.90959999999999996</v>
       </c>
       <c r="DR12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.98052858129423781</v>
       </c>
       <c r="DT12" s="2">
         <v>0.6</v>
       </c>
       <c r="DU12" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>6.8436389110394E-2</v>
       </c>
       <c r="DV12" s="2">
         <v>1.0135000000000001</v>
       </c>
       <c r="DW12">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.97832870538154948</v>
       </c>
       <c r="DY12" s="2">
         <v>0.6</v>
       </c>
       <c r="DZ12" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>6.8493661099363778E-2</v>
       </c>
       <c r="EA12" s="2">
         <v>0.81730000000000003</v>
       </c>
       <c r="EB12">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0.98248699899859548</v>
       </c>
       <c r="ED12" s="2">
         <v>5.8010000000000002</v>
       </c>
       <c r="EE12" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>0.37377294330768335</v>
       </c>
       <c r="EF12" s="2">
         <v>1.35</v>
       </c>
       <c r="EG12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.75415303213518359</v>
       </c>
       <c r="EI12" s="2">
         <v>3.9580000000000002</v>
       </c>
       <c r="EJ12" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.372357869843366</v>
       </c>
       <c r="EK12" s="2">
         <v>1.34</v>
       </c>
       <c r="EL12">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0.82605773211349576</v>
       </c>
       <c r="EN12" s="2">
         <v>3.81</v>
       </c>
       <c r="EO12" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0.31195343300834599</v>
       </c>
       <c r="EP12" s="2">
         <v>0.97</v>
       </c>
       <c r="EQ12">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.87532994246531504</v>
       </c>
       <c r="ES12" s="2">
         <v>5.9960000000000004</v>
       </c>
       <c r="ET12" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>0.42030206065458381</v>
       </c>
       <c r="EU12" s="2">
         <v>1.07</v>
       </c>
       <c r="EV12">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.7936160749499328</v>
       </c>
       <c r="EX12" s="2">
         <v>4.32</v>
       </c>
       <c r="EY12" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.47898735148013444</v>
       </c>
       <c r="EZ12" s="2">
         <v>0.79</v>
       </c>
       <c r="FA12">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.88429759370363636</v>
       </c>
       <c r="FC12" s="2">
@@ -6805,14 +6805,14 @@
         <v>3.0219999999999998</v>
       </c>
       <c r="FI12" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.37658486932327373</v>
       </c>
       <c r="FJ12" s="2">
         <v>2.06</v>
       </c>
       <c r="FK12">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>0.79907901777861967</v>
       </c>
       <c r="FM12" s="2">
@@ -6833,42 +6833,42 @@
         <v>1.7969999999999999</v>
       </c>
       <c r="FS12" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>0.22171624006041163</v>
       </c>
       <c r="FT12" s="2">
         <v>1.35</v>
       </c>
       <c r="FU12">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>0.9163051168124039</v>
       </c>
       <c r="FW12" s="2">
         <v>1.996</v>
       </c>
       <c r="FX12" s="2">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>0.33059783477317722</v>
       </c>
       <c r="FY12" s="2">
         <v>1.54</v>
       </c>
       <c r="FZ12">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0.89516335820863435</v>
       </c>
       <c r="GB12" s="2">
         <v>2.37</v>
       </c>
       <c r="GC12" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.44726618129636092</v>
       </c>
       <c r="GD12" s="2">
         <v>1.79</v>
       </c>
       <c r="GE12">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0.85826005117329662</v>
       </c>
       <c r="GG12" s="2">
@@ -6889,14 +6889,14 @@
         <v>1.8879999999999999</v>
       </c>
       <c r="GM12" s="2">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0.35938514093321899</v>
       </c>
       <c r="GN12" s="2">
         <v>1.34</v>
       </c>
       <c r="GO12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0.91287906642256578</v>
       </c>
       <c r="GQ12" s="2">
@@ -7130,7 +7130,7 @@
         <v>0.7</v>
       </c>
       <c r="CR13" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="47"/>
         <v>0.10049780070812771</v>
       </c>
       <c r="CS13" s="2">
@@ -7140,7 +7140,7 @@
         <v>0.7</v>
       </c>
       <c r="CV13" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.10153533056878149</v>
       </c>
       <c r="CW13" s="2">
@@ -7150,7 +7150,7 @@
         <v>1</v>
       </c>
       <c r="CZ13" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>6.4511300703487498E-2</v>
       </c>
       <c r="DA13" s="2">
@@ -7160,7 +7160,7 @@
         <v>1</v>
       </c>
       <c r="DD13" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>9.1817273635455457E-2</v>
       </c>
       <c r="DE13" s="2">
@@ -7170,7 +7170,7 @@
         <v>1</v>
       </c>
       <c r="DL13" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.14096727085301949</v>
       </c>
       <c r="DM13" s="2">
@@ -7187,105 +7187,105 @@
         <v>0.91</v>
       </c>
       <c r="DR13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.97731054704451703</v>
       </c>
       <c r="DT13" s="2">
         <v>0.7</v>
       </c>
       <c r="DU13" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>7.8942035980208311E-2</v>
       </c>
       <c r="DV13" s="2">
         <v>1.0285</v>
       </c>
       <c r="DW13">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.97439406754034741</v>
       </c>
       <c r="DY13" s="2">
         <v>0.7</v>
       </c>
       <c r="DZ13" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>7.9007354126277282E-2</v>
       </c>
       <c r="EA13" s="2">
         <v>0.80169999999999997</v>
       </c>
       <c r="EB13">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0.97998362178217957</v>
       </c>
       <c r="ED13" s="2">
         <v>7.9809999999999999</v>
       </c>
       <c r="EE13" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>0.45090096142793945</v>
       </c>
       <c r="EF13" s="2">
         <v>1.7</v>
       </c>
       <c r="EG13">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.61333865086347206</v>
       </c>
       <c r="EI13" s="2">
         <v>5.0730000000000004</v>
       </c>
       <c r="EJ13" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.43194469354458598</v>
       </c>
       <c r="EK13" s="2">
         <v>1.47</v>
       </c>
       <c r="EL13">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0.76438516020631775</v>
       </c>
       <c r="EN13" s="2">
         <v>4.3490000000000002</v>
       </c>
       <c r="EO13" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0.34103487836492302</v>
       </c>
       <c r="EP13" s="2">
         <v>1.17</v>
       </c>
       <c r="EQ13">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.83249321211796445</v>
       </c>
       <c r="ES13" s="2">
         <v>6.9489999999999998</v>
       </c>
       <c r="ET13" s="2">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>0.45660238642408441</v>
       </c>
       <c r="EU13" s="2">
         <v>1.19</v>
       </c>
       <c r="EV13">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.74234627233627271</v>
       </c>
       <c r="EX13" s="2">
         <v>5.8879999999999999</v>
       </c>
       <c r="EY13" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.5561523393115233</v>
       </c>
       <c r="EZ13" s="2">
         <v>0.78</v>
       </c>
       <c r="FA13">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.84749467240479803</v>
       </c>
       <c r="FF13"/>
@@ -7293,70 +7293,70 @@
         <v>3.3759999999999999</v>
       </c>
       <c r="FI13" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.40292399107767829</v>
       </c>
       <c r="FJ13" s="2">
         <v>2.21</v>
       </c>
       <c r="FK13" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>0.76428464417717057</v>
       </c>
       <c r="FR13" s="2">
         <v>2.2130000000000001</v>
       </c>
       <c r="FS13" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>0.25971269345992959</v>
       </c>
       <c r="FT13" s="2">
         <v>1.39</v>
       </c>
       <c r="FU13" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>0.89509143840689942</v>
       </c>
       <c r="FW13" s="2">
         <v>2.395</v>
       </c>
       <c r="FX13" s="2">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>0.37209391327618574</v>
       </c>
       <c r="FY13" s="2">
         <v>1.62</v>
       </c>
       <c r="FZ13" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0.86953992535188906</v>
       </c>
       <c r="GB13" s="2">
         <v>2.9329999999999998</v>
       </c>
       <c r="GC13" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.50035329768497339</v>
       </c>
       <c r="GD13" s="2">
         <v>1.96</v>
       </c>
       <c r="GE13" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0.81292020725998193</v>
       </c>
       <c r="GL13" s="2">
         <v>2.2450000000000001</v>
       </c>
       <c r="GM13" s="2">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0.40014851123158923</v>
       </c>
       <c r="GN13" s="2">
         <v>1.37</v>
       </c>
       <c r="GO13" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0.89510498339874134</v>
       </c>
       <c r="GQ13" s="2">
@@ -7575,7 +7575,7 @@
         <v>0.8</v>
       </c>
       <c r="CR14" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="47"/>
         <v>0.11322901974349477</v>
       </c>
       <c r="CS14" s="2">
@@ -7585,7 +7585,7 @@
         <v>0.8</v>
       </c>
       <c r="CV14" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.11438127204039329</v>
       </c>
       <c r="CW14" s="2">
@@ -7595,7 +7595,7 @@
         <v>1.5</v>
       </c>
       <c r="CZ14" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>9.3743203074023049E-2</v>
       </c>
       <c r="DA14" s="2">
@@ -7605,7 +7605,7 @@
         <v>1.5</v>
       </c>
       <c r="DD14" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>0.1316806321364998</v>
       </c>
       <c r="DE14" s="2">
@@ -7615,7 +7615,7 @@
         <v>1.5</v>
       </c>
       <c r="DL14" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.19752838743329451</v>
       </c>
       <c r="DM14" s="2">
@@ -7632,21 +7632,21 @@
         <v>0.91100000000000003</v>
       </c>
       <c r="DR14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.97408342034845929</v>
       </c>
       <c r="DT14" s="2">
         <v>0.8</v>
       </c>
       <c r="DU14" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>8.9213371804960501E-2</v>
       </c>
       <c r="DV14" s="2">
         <v>0.91100000000000003</v>
       </c>
       <c r="DW14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.97408342034845929</v>
       </c>
       <c r="EB14"/>
@@ -7654,84 +7654,84 @@
         <v>6.6929999999999996</v>
       </c>
       <c r="EJ14" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.50080215353152246</v>
       </c>
       <c r="EK14" s="2">
         <v>1.66</v>
       </c>
       <c r="EL14" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0.67011768847610276</v>
       </c>
       <c r="FH14" s="2">
         <v>3.9489999999999998</v>
       </c>
       <c r="FI14" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.44114271873147265</v>
       </c>
       <c r="FJ14" s="2">
         <v>2.4500000000000002</v>
       </c>
       <c r="FK14" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>0.70568406484515256</v>
       </c>
       <c r="FR14" s="2">
         <v>2.6930000000000001</v>
       </c>
       <c r="FS14" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>0.29919049704556583</v>
       </c>
       <c r="FT14" s="2">
         <v>1.54</v>
       </c>
       <c r="FU14" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>0.86120522499020669</v>
       </c>
       <c r="FW14" s="2">
         <v>2.6560000000000001</v>
       </c>
       <c r="FX14" s="2">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>0.39656309372157211</v>
       </c>
       <c r="FY14" s="2">
         <v>1.81</v>
       </c>
       <c r="FZ14" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0.8409635260134265</v>
       </c>
       <c r="GB14" s="2">
         <v>3.5169999999999999</v>
       </c>
       <c r="GC14" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.54562169677481054</v>
       </c>
       <c r="GD14" s="2">
         <v>2.2599999999999998</v>
       </c>
       <c r="GE14" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0.75097872995281467</v>
       </c>
       <c r="GL14" s="2">
         <v>2.5030000000000001</v>
       </c>
       <c r="GM14" s="2">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0.42652047572512208</v>
       </c>
       <c r="GN14" s="2">
         <v>1.42</v>
       </c>
       <c r="GO14" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0.87980202548305697</v>
       </c>
       <c r="GQ14" s="2">
@@ -7947,7 +7947,7 @@
         <v>0.9</v>
       </c>
       <c r="CR15" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="47"/>
         <v>0.12560488249642324</v>
       </c>
       <c r="CS15" s="2">
@@ -7957,7 +7957,7 @@
         <v>0.9</v>
       </c>
       <c r="CV15" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.12686505771063983</v>
       </c>
       <c r="CW15" s="2">
@@ -7967,7 +7967,7 @@
         <v>2</v>
       </c>
       <c r="CZ15" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0.12120359955005623</v>
       </c>
       <c r="DA15" s="2">
@@ -7977,7 +7977,7 @@
         <v>2</v>
       </c>
       <c r="DD15" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>0.1681916486441524</v>
       </c>
       <c r="DE15" s="2">
@@ -7987,7 +7987,7 @@
         <v>2</v>
       </c>
       <c r="DL15" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.24710134015961449</v>
       </c>
       <c r="DM15" s="2">
@@ -8004,21 +8004,21 @@
         <v>0.91220000000000001</v>
       </c>
       <c r="DR15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.97085365751222485</v>
       </c>
       <c r="DT15" s="2">
         <v>0.9</v>
       </c>
       <c r="DU15" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>9.9258149011525895E-2</v>
       </c>
       <c r="DV15" s="2">
         <v>0.91220000000000001</v>
       </c>
       <c r="DW15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.97085365751222485</v>
       </c>
       <c r="EB15"/>
@@ -8026,84 +8026,84 @@
         <v>8.3979999999999997</v>
       </c>
       <c r="EJ15" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.55728239426922954</v>
       </c>
       <c r="EK15" s="2">
         <v>1.8</v>
       </c>
       <c r="EL15" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0.58005230275597131</v>
       </c>
       <c r="FH15" s="2">
         <v>4.5960000000000001</v>
       </c>
       <c r="FI15" s="2">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>0.47881226986825476</v>
       </c>
       <c r="FJ15" s="2">
         <v>2.7</v>
       </c>
       <c r="FK15" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>0.63948135101347503</v>
       </c>
       <c r="FR15" s="2">
         <v>3.2029999999999998</v>
       </c>
       <c r="FS15" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>0.33676956998506646</v>
       </c>
       <c r="FT15" s="2">
         <v>1.87</v>
       </c>
       <c r="FU15" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>0.80589411313039805</v>
       </c>
       <c r="FW15" s="2">
         <v>3.34</v>
       </c>
       <c r="FX15" s="2">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>0.45247967029639791</v>
       </c>
       <c r="FY15" s="2">
         <v>2.09</v>
       </c>
       <c r="FZ15" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0.7776273637667005</v>
       </c>
       <c r="GB15" s="2">
         <v>4.1559999999999997</v>
       </c>
       <c r="GC15" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>0.58660314399553382</v>
       </c>
       <c r="GD15" s="2">
         <v>2.59</v>
       </c>
       <c r="GE15" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>0.6785321239859966</v>
       </c>
       <c r="GL15" s="2">
         <v>3.3980000000000001</v>
       </c>
       <c r="GM15" s="2">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>0.50240876948415492</v>
       </c>
       <c r="GN15" s="2">
         <v>1.6</v>
       </c>
       <c r="GO15" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>0.82210642126294919</v>
       </c>
       <c r="GQ15" s="2">
@@ -8306,7 +8306,7 @@
         <v>1</v>
       </c>
       <c r="CR16" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="47"/>
         <v>0.13764006234517406</v>
       </c>
       <c r="CS16" s="2">
@@ -8316,7 +8316,7 @@
         <v>1</v>
       </c>
       <c r="CV16" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.13900178967087998</v>
       </c>
       <c r="CW16" s="2">
@@ -8326,7 +8326,7 @@
         <v>2.5</v>
       </c>
       <c r="CZ16" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0.1470487888092801</v>
       </c>
       <c r="DA16" s="2">
@@ -8336,7 +8336,7 @@
         <v>2.5</v>
       </c>
       <c r="DD16" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>0.20175613649970064</v>
       </c>
       <c r="DE16" s="2">
@@ -8346,7 +8346,7 @@
         <v>2.5</v>
       </c>
       <c r="DL16" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.29090586775394434</v>
       </c>
       <c r="DM16" s="2">
@@ -8363,21 +8363,21 @@
         <v>0.91349999999999998</v>
       </c>
       <c r="DR16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.96762275008731913</v>
       </c>
       <c r="DT16" s="2">
         <v>1</v>
       </c>
       <c r="DU16" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.10908378176116316</v>
       </c>
       <c r="DV16" s="2">
         <v>0.91349999999999998</v>
       </c>
       <c r="DW16">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.96762275008731913</v>
       </c>
       <c r="EB16"/>
@@ -8584,7 +8584,7 @@
         <v>1.2</v>
       </c>
       <c r="CR17" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="47"/>
         <v>0.16074313576846283</v>
       </c>
       <c r="CS17" s="2">
@@ -8594,7 +8594,7 @@
         <v>1.2</v>
       </c>
       <c r="CV17" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.16229041595229585</v>
       </c>
       <c r="CW17" s="2">
@@ -8604,7 +8604,7 @@
         <v>3</v>
       </c>
       <c r="CZ17" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0.1714172080074241</v>
       </c>
       <c r="DA17" s="2">
@@ -8614,7 +8614,7 @@
         <v>3</v>
       </c>
       <c r="DD17" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>0.23271694928259035</v>
       </c>
       <c r="DE17" s="2">
@@ -8624,7 +8624,7 @@
         <v>3</v>
       </c>
       <c r="DL17" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.32989345305903639</v>
       </c>
       <c r="DM17" s="2">
@@ -8641,21 +8641,21 @@
         <v>0.91659999999999997</v>
       </c>
       <c r="DR17">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.96114536582444166</v>
       </c>
       <c r="DT17" s="2">
         <v>1.2</v>
       </c>
       <c r="DU17" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.12810568754097901</v>
       </c>
       <c r="DV17" s="2">
         <v>0.91659999999999997</v>
       </c>
       <c r="DW17">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.96114536582444166</v>
       </c>
       <c r="EB17"/>
@@ -8840,7 +8840,7 @@
         <v>1.4</v>
       </c>
       <c r="CR18" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="47"/>
         <v>0.18264062071448259</v>
       </c>
       <c r="CS18" s="2">
@@ -8850,7 +8850,7 @@
         <v>1.4</v>
       </c>
       <c r="CV18" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.18435238117392636</v>
       </c>
       <c r="CW18" s="2">
@@ -8860,7 +8860,7 @@
         <v>3.5</v>
       </c>
       <c r="CZ18" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0.19443191338531929</v>
       </c>
       <c r="DA18" s="2">
@@ -8870,7 +8870,7 @@
         <v>3.5</v>
       </c>
       <c r="DD18" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>0.26136573475643538</v>
       </c>
       <c r="DE18" s="2">
@@ -8880,7 +8880,7 @@
         <v>3.5</v>
       </c>
       <c r="DL18" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.36481722615682666</v>
       </c>
       <c r="DM18" s="2">
@@ -8897,21 +8897,21 @@
         <v>0.92020000000000002</v>
       </c>
       <c r="DR18">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.95464461253083843</v>
       </c>
       <c r="DT18" s="2">
         <v>1.4</v>
       </c>
       <c r="DU18" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.14633230210275425</v>
       </c>
       <c r="DV18" s="2">
         <v>0.92020000000000002</v>
       </c>
       <c r="DW18">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.95464461253083843</v>
       </c>
       <c r="EB18"/>
@@ -9108,7 +9108,7 @@
         <v>1.6</v>
       </c>
       <c r="CV19" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.2052821146769008</v>
       </c>
       <c r="CW19" s="2">
@@ -9118,7 +9118,7 @@
         <v>4</v>
       </c>
       <c r="CZ19" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0.21620265864058186</v>
       </c>
       <c r="DA19" s="2">
@@ -9128,7 +9128,7 @@
         <v>4</v>
       </c>
       <c r="DL19" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.39628109152378649</v>
       </c>
       <c r="DM19" s="2">
@@ -9145,21 +9145,21 @@
         <v>0.9244</v>
       </c>
       <c r="DR19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.9481058402815703</v>
       </c>
       <c r="DT19" s="2">
         <v>1.6</v>
       </c>
       <c r="DU19" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.1638124799314995</v>
       </c>
       <c r="DV19" s="2">
         <v>0.9244</v>
       </c>
       <c r="DW19">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.9481058402815703</v>
       </c>
       <c r="GQ19" s="2">
@@ -9333,7 +9333,7 @@
         <v>1.8</v>
       </c>
       <c r="CV20" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.22516459596037394</v>
       </c>
       <c r="CW20" s="2">
@@ -9343,7 +9343,7 @@
         <v>4.5</v>
       </c>
       <c r="CZ20" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0.23682764515538191</v>
       </c>
       <c r="DA20" s="2">
@@ -9353,7 +9353,7 @@
         <v>4.5</v>
       </c>
       <c r="DL20" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.42477494319652565</v>
       </c>
       <c r="DM20" s="2">
@@ -9370,21 +9370,21 @@
         <v>0.92900000000000005</v>
       </c>
       <c r="DR20">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.94153043639048362</v>
       </c>
       <c r="DT20" s="2">
         <v>1.8</v>
       </c>
       <c r="DU20" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.18059115431762909</v>
       </c>
       <c r="DV20" s="2">
         <v>0.92900000000000005</v>
       </c>
       <c r="DW20">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.94153043639048362</v>
       </c>
       <c r="GQ20" s="2">
@@ -9502,7 +9502,7 @@
         <v>2</v>
       </c>
       <c r="CV21" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.24407650792374122</v>
       </c>
       <c r="CW21" s="2">
@@ -9512,7 +9512,7 @@
         <v>5</v>
       </c>
       <c r="DL21" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.45070035704476791</v>
       </c>
       <c r="DM21" s="2">
@@ -9529,21 +9529,21 @@
         <v>0.93379999999999996</v>
       </c>
       <c r="DR21">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.93492517765215333</v>
       </c>
       <c r="DT21" s="2">
         <v>2</v>
       </c>
       <c r="DU21" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.19670972302551248</v>
       </c>
       <c r="DV21" s="2">
         <v>0.93379999999999996</v>
       </c>
       <c r="DW21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.93492517765215333</v>
       </c>
       <c r="GQ21" s="2">
@@ -9661,7 +9661,7 @@
         <v>2.5</v>
       </c>
       <c r="CV22" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.28754960881130143</v>
       </c>
       <c r="CW22" s="2">
@@ -9681,7 +9681,7 @@
         <v>5.5</v>
       </c>
       <c r="DL22" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.47438963496360148</v>
       </c>
       <c r="DM22" s="2">
@@ -9698,21 +9698,21 @@
         <v>0.94450000000000001</v>
       </c>
       <c r="DR22">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.92157439663809559</v>
       </c>
       <c r="DT22" s="2">
         <v>2.4</v>
       </c>
       <c r="DU22" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.22711646427423143</v>
       </c>
       <c r="DV22" s="2">
         <v>0.94450000000000001</v>
       </c>
       <c r="DW22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.92157439663809559</v>
       </c>
     </row>
@@ -9813,7 +9813,7 @@
         <v>3</v>
       </c>
       <c r="CV23" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.32629436705288412</v>
       </c>
       <c r="CW23" s="11">
@@ -9833,7 +9833,7 @@
         <v>6</v>
       </c>
       <c r="DL23" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.49612012496220897</v>
       </c>
       <c r="DM23" s="2">
@@ -9850,21 +9850,21 @@
         <v>0.95279999999999998</v>
       </c>
       <c r="DR23">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.91147768727147049</v>
       </c>
       <c r="DT23" s="2">
         <v>2.7</v>
       </c>
       <c r="DU23" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.24845256382892372</v>
       </c>
       <c r="DV23" s="2">
         <v>0.95279999999999998</v>
       </c>
       <c r="DW23">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.91147768727147049</v>
       </c>
     </row>
@@ -9934,21 +9934,21 @@
         <v>0.96179999999999999</v>
       </c>
       <c r="DR24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.90126166538009622</v>
       </c>
       <c r="DT24" s="2">
         <v>3</v>
       </c>
       <c r="DU24" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.26864230757979113</v>
       </c>
       <c r="DV24" s="2">
         <v>0.96179999999999999</v>
       </c>
       <c r="DW24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.90126166538009622</v>
       </c>
     </row>
@@ -10008,21 +10008,21 @@
         <v>0.97419999999999995</v>
       </c>
       <c r="DR25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.88750605177911046</v>
       </c>
       <c r="DT25" s="2">
         <v>3.4</v>
       </c>
       <c r="DU25" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.29393290668052435</v>
       </c>
       <c r="DV25" s="2">
         <v>0.97419999999999995</v>
       </c>
       <c r="DW25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.88750605177911046</v>
       </c>
     </row>
@@ -10060,21 +10060,21 @@
         <v>0.98360000000000003</v>
       </c>
       <c r="DR26">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.87710984737211428</v>
       </c>
       <c r="DT26" s="2">
         <v>3.7</v>
       </c>
       <c r="DU26" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.31178201658880628</v>
       </c>
       <c r="DV26" s="2">
         <v>0.98360000000000003</v>
       </c>
       <c r="DW26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.87710984737211428</v>
       </c>
     </row>
@@ -10112,21 +10112,21 @@
         <v>0.99250000000000005</v>
       </c>
       <c r="DR27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.8667217477376794</v>
       </c>
       <c r="DT27" s="2">
         <v>4</v>
       </c>
       <c r="DU27" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.32875093974868436</v>
       </c>
       <c r="DV27" s="2">
         <v>0.99250000000000005</v>
       </c>
       <c r="DW27">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.8667217477376794</v>
       </c>
     </row>
@@ -10164,21 +10164,21 @@
         <v>1.0089999999999999</v>
       </c>
       <c r="DR28">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.8490882556844872</v>
       </c>
       <c r="DT28" s="2">
         <v>4.5</v>
       </c>
       <c r="DU28" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.35524636036570428</v>
       </c>
       <c r="DV28" s="2">
         <v>1.0089999999999999</v>
       </c>
       <c r="DW28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.8490882556844872</v>
       </c>
     </row>
@@ -10216,21 +10216,21 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="DR29">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.83139404553783947</v>
       </c>
       <c r="DT29" s="2">
         <v>5</v>
       </c>
       <c r="DU29" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.37972956208907077</v>
       </c>
       <c r="DV29" s="2">
         <v>1.0249999999999999</v>
       </c>
       <c r="DW29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.83139404553783947</v>
       </c>
     </row>
@@ -10268,21 +10268,21 @@
         <v>1.0411999999999999</v>
       </c>
       <c r="DR30">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.81356716887718761</v>
       </c>
       <c r="DT30" s="2">
         <v>5.5</v>
       </c>
       <c r="DU30" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.40242138853366155</v>
       </c>
       <c r="DV30" s="2">
         <v>1.0411999999999999</v>
       </c>
       <c r="DW30">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.81356716887718761</v>
       </c>
     </row>
@@ -10320,21 +10320,21 @@
         <v>1.0569999999999999</v>
       </c>
       <c r="DR31">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.79572679892361964</v>
       </c>
       <c r="DT31" s="2">
         <v>6</v>
       </c>
       <c r="DU31" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.42351150671032606</v>
       </c>
       <c r="DV31" s="2">
         <v>1.0569999999999999</v>
       </c>
       <c r="DW31">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.79572679892361964</v>
       </c>
     </row>
@@ -10372,21 +10372,21 @@
         <v>1.0745</v>
       </c>
       <c r="DR32">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.77752510639851602</v>
       </c>
       <c r="DT32" s="2">
         <v>6.5</v>
       </c>
       <c r="DU32" s="2">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.44316372100275075</v>
       </c>
       <c r="DV32" s="2">
         <v>1.0745</v>
       </c>
       <c r="DW32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>0.77752510639851602</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reorganize and add MgCL2 simulations
</commit_message>
<xml_diff>
--- a/data/sources_list_.xlsx
+++ b/data/sources_list_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/peterbaz_stanford_edu/Documents/DiazMarin2026/hygroscopic-salts-main/hygroscopic-salts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="324" documentId="13_ncr:1_{B1905FFE-40A5-1548-B975-09D0200E2583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C77F5915-02D9-49E9-ACDB-8363D46C9911}"/>
+  <xr:revisionPtr revIDLastSave="327" documentId="13_ncr:1_{B1905FFE-40A5-1548-B975-09D0200E2583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8420147E-298E-438C-B9E9-FF5A4EF8E1F6}"/>
   <bookViews>
-    <workbookView xWindow="14160" yWindow="480" windowWidth="19560" windowHeight="19485" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8538" yWindow="3186" windowWidth="13224" windowHeight="9444" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sources" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="417">
   <si>
     <t xml:space="preserve">Data Source </t>
   </si>
@@ -1284,6 +1284,9 @@
   </si>
   <si>
     <t>notused</t>
+  </si>
+  <si>
+    <t>Deliquescence limits</t>
   </si>
 </sst>
 </file>
@@ -2131,15 +2134,15 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="25.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="4" width="25.42578125" style="2" customWidth="1"/>
-    <col min="5" max="8" width="13.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="25.42578125" style="2"/>
+    <col min="1" max="4" width="25.41796875" style="2" customWidth="1"/>
+    <col min="5" max="8" width="13.15625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="25.41796875" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="25.41796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2171,7 +2174,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -2203,7 +2206,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -2232,7 +2235,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -2252,7 +2255,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -2275,7 +2278,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
@@ -2289,7 +2292,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
@@ -2300,7 +2303,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4" t="s">
         <v>46</v>
       </c>
@@ -2343,7 +2346,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="159.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="160" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
         <v>53</v>
       </c>
@@ -2372,7 +2375,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4" t="s">
         <v>60</v>
       </c>
@@ -2395,10 +2398,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
         <v>65</v>
       </c>
@@ -2412,7 +2415,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4" t="s">
         <v>68</v>
       </c>
@@ -2433,7 +2436,7 @@
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4" t="s">
         <v>73</v>
       </c>
@@ -2442,7 +2445,7 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4" t="s">
         <v>74</v>
       </c>
@@ -2450,12 +2453,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4" t="s">
         <v>76</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
         <v>83</v>
       </c>
@@ -2507,10 +2510,10 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
     </row>
@@ -2544,18 +2547,18 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="25.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="25.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="2" customWidth="1"/>
-    <col min="7" max="9" width="13.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="25.42578125" style="2"/>
+    <col min="1" max="3" width="25.41796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.41796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.41796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.41796875" style="2" customWidth="1"/>
+    <col min="7" max="9" width="13.15625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="25.41796875" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="25.41796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -2578,7 +2581,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>95</v>
       </c>
@@ -2595,7 +2598,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>98</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>101</v>
       </c>
@@ -2632,7 +2635,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4" t="s">
         <v>104</v>
       </c>
@@ -2649,7 +2652,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="320.10000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="320.10000000000002" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
         <v>107</v>
       </c>
@@ -2669,7 +2672,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
         <v>110</v>
       </c>
@@ -2686,10 +2689,10 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:9" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4" t="s">
         <v>113</v>
       </c>
@@ -2706,7 +2709,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
         <v>116</v>
       </c>
@@ -2729,7 +2732,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="64" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4" t="s">
         <v>121</v>
       </c>
@@ -2758,7 +2761,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4" t="s">
         <v>126</v>
       </c>
@@ -2781,7 +2784,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4" t="s">
         <v>405</v>
       </c>
@@ -2798,7 +2801,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4" t="s">
         <v>408</v>
       </c>
@@ -2847,15 +2850,15 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="25.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="25.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="25.42578125" style="2"/>
+    <col min="1" max="2" width="25.41796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.15625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.41796875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="25.41796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>90</v>
       </c>
@@ -2866,7 +2869,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="32.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>130</v>
       </c>
@@ -2874,7 +2877,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="111.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="112" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>131</v>
       </c>
@@ -2885,7 +2888,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>132</v>
       </c>
@@ -2896,7 +2899,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
         <v>404</v>
       </c>
@@ -2907,7 +2910,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4" t="s">
         <v>386</v>
       </c>
@@ -2918,7 +2921,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>388</v>
       </c>
@@ -2929,7 +2932,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4" t="s">
         <v>392</v>
       </c>
@@ -2940,7 +2943,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
         <v>394</v>
       </c>
@@ -2951,7 +2954,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4" t="s">
         <v>396</v>
       </c>
@@ -2962,7 +2965,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="9" t="s">
         <v>397</v>
       </c>
@@ -2973,7 +2976,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="9" t="s">
         <v>399</v>
       </c>
@@ -2984,7 +2987,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="9" t="s">
         <v>401</v>
       </c>
@@ -2998,7 +3001,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="9" t="s">
         <v>405</v>
       </c>
@@ -3009,7 +3012,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="9" t="s">
         <v>410</v>
       </c>
@@ -3020,7 +3023,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
         <v>412</v>
       </c>
@@ -3056,24 +3059,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:GS34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BG1" zoomScale="75" zoomScaleNormal="32" workbookViewId="0">
-      <selection activeCell="BL4" sqref="BL4"/>
+    <sheetView tabSelected="1" topLeftCell="EI7" zoomScale="75" zoomScaleNormal="32" workbookViewId="0">
+      <selection activeCell="DZ1" sqref="DZ1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="48.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.41796875" defaultRowHeight="49" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="7.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="20.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.42578125" style="2" customWidth="1"/>
-    <col min="8" max="13" width="8.42578125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.42578125" style="6" customWidth="1"/>
-    <col min="15" max="308" width="8.42578125" style="2" customWidth="1"/>
-    <col min="309" max="16384" width="20.42578125" style="2"/>
+    <col min="1" max="1" width="20.41796875" style="2" customWidth="1"/>
+    <col min="2" max="3" width="7.41796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.41796875" style="2" customWidth="1"/>
+    <col min="5" max="6" width="20.41796875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.41796875" style="2" customWidth="1"/>
+    <col min="8" max="13" width="8.41796875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.41796875" style="6" customWidth="1"/>
+    <col min="15" max="308" width="8.41796875" style="2" customWidth="1"/>
+    <col min="309" max="16384" width="20.41796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:201" s="1" customFormat="1" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:201" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -3258,8 +3261,11 @@
       <c r="DW1" s="8" t="s">
         <v>155</v>
       </c>
+      <c r="DY1" s="1" t="s">
+        <v>416</v>
+      </c>
     </row>
-    <row r="2" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>90</v>
       </c>
@@ -3450,7 +3456,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>175</v>
       </c>
@@ -3627,7 +3633,7 @@
         <v>8.0043000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>180</v>
       </c>
@@ -3778,7 +3784,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="5" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="S5" s="2" t="s">
         <v>207</v>
       </c>
@@ -3804,7 +3810,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>209</v>
       </c>
@@ -3911,7 +3917,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="O7" s="2">
         <v>0.1</v>
       </c>
@@ -4364,7 +4370,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>251</v>
       </c>
@@ -4882,7 +4888,7 @@
         <v>0.73199999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4" t="s">
         <v>258</v>
       </c>
@@ -5102,7 +5108,7 @@
         <v>0.3</v>
       </c>
       <c r="CR9" s="2">
-        <f t="shared" ref="CR8:CR18" si="47">$BW$3*CQ9/(1+$BW$3*CQ9)</f>
+        <f t="shared" ref="CR9:CR18" si="47">$BW$3*CQ9/(1+$BW$3*CQ9)</f>
         <v>4.5694604446998244E-2</v>
       </c>
       <c r="CS9" s="2">
@@ -5393,7 +5399,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="O10" s="2">
         <v>3</v>
       </c>
@@ -5895,7 +5901,7 @@
         <v>0.70599999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4" t="s">
         <v>267</v>
       </c>
@@ -6409,7 +6415,7 @@
         <v>0.69699999999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4" t="s">
         <v>275</v>
       </c>
@@ -6910,7 +6916,7 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="13" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4" t="s">
         <v>284</v>
       </c>
@@ -7370,7 +7376,7 @@
         <v>0.67600000000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4" t="s">
         <v>290</v>
       </c>
@@ -7745,7 +7751,7 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4" t="s">
         <v>297</v>
       </c>
@@ -8117,7 +8123,7 @@
         <v>0.65400000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4" t="s">
         <v>304</v>
       </c>
@@ -8392,7 +8398,7 @@
         <v>0.64500000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4" t="s">
         <v>312</v>
       </c>
@@ -8670,7 +8676,7 @@
         <v>0.629</v>
       </c>
     </row>
-    <row r="18" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="V18" s="2">
         <v>5</v>
       </c>
@@ -8926,7 +8932,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="19" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
         <v>324</v>
       </c>
@@ -9173,7 +9179,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4" t="s">
         <v>331</v>
       </c>
@@ -9398,7 +9404,7 @@
         <v>0.39200000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4" t="s">
         <v>337</v>
       </c>
@@ -9557,7 +9563,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4" t="s">
         <v>341</v>
       </c>
@@ -9716,7 +9722,7 @@
         <v>0.92157439663809559</v>
       </c>
     </row>
-    <row r="23" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>350</v>
       </c>
@@ -9868,7 +9874,7 @@
         <v>0.91147768727147049</v>
       </c>
     </row>
-    <row r="24" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="9" t="s">
         <v>352</v>
       </c>
@@ -9952,7 +9958,7 @@
         <v>0.90126166538009622</v>
       </c>
     </row>
-    <row r="25" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>383</v>
       </c>
@@ -10026,7 +10032,7 @@
         <v>0.88750605177911046</v>
       </c>
     </row>
-    <row r="26" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX26" s="2">
         <v>7.4950000000000001</v>
       </c>
@@ -10078,7 +10084,7 @@
         <v>0.87710984737211428</v>
       </c>
     </row>
-    <row r="27" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX27" s="2">
         <v>7.9480000000000004</v>
       </c>
@@ -10130,7 +10136,7 @@
         <v>0.8667217477376794</v>
       </c>
     </row>
-    <row r="28" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX28" s="2">
         <v>7.9969999999999999</v>
       </c>
@@ -10182,7 +10188,7 @@
         <v>0.8490882556844872</v>
       </c>
     </row>
-    <row r="29" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX29" s="2">
         <v>8.9870000000000001</v>
       </c>
@@ -10234,7 +10240,7 @@
         <v>0.83139404553783947</v>
       </c>
     </row>
-    <row r="30" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX30" s="2">
         <v>9.9670000000000005</v>
       </c>
@@ -10286,7 +10292,7 @@
         <v>0.81356716887718761</v>
       </c>
     </row>
-    <row r="31" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX31" s="2">
         <v>11.013</v>
       </c>
@@ -10338,7 +10344,7 @@
         <v>0.79572679892361964</v>
       </c>
     </row>
-    <row r="32" spans="1:201" ht="48.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX32" s="2">
         <v>11.999000000000001</v>
       </c>
@@ -10390,8 +10396,8 @@
         <v>0.77752510639851602</v>
       </c>
     </row>
-    <row r="33" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="14.4" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="34" ht="14.4" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="BG1" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>

</xml_diff>

<commit_message>
Add AN data, fix salts using osmotic coeff. RH limits have changed
</commit_message>
<xml_diff>
--- a/data/sources_list_.xlsx
+++ b/data/sources_list_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://office365stanford-my.sharepoint.com/personal/peterbaz_stanford_edu/Documents/DiazMarin2026/hygroscopic-salts-main/hygroscopic-salts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="327" documentId="13_ncr:1_{B1905FFE-40A5-1548-B975-09D0200E2583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8420147E-298E-438C-B9E9-FF5A4EF8E1F6}"/>
+  <xr:revisionPtr revIDLastSave="487" documentId="13_ncr:1_{B1905FFE-40A5-1548-B975-09D0200E2583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50822A1E-8030-415A-B182-4B98766878BD}"/>
   <bookViews>
-    <workbookView xWindow="8538" yWindow="3186" windowWidth="13224" windowHeight="9444" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9222" yWindow="930" windowWidth="13116" windowHeight="10650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Sources" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="418">
   <si>
     <t xml:space="preserve">Data Source </t>
   </si>
@@ -1287,6 +1287,9 @@
   </si>
   <si>
     <t>Deliquescence limits</t>
+  </si>
+  <si>
+    <t>mass fraction</t>
   </si>
 </sst>
 </file>
@@ -1807,10 +1810,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3057,10 +3056,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:GS34"/>
+  <dimension ref="A1:GV34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EI7" zoomScale="75" zoomScaleNormal="32" workbookViewId="0">
-      <selection activeCell="DZ1" sqref="DZ1"/>
+    <sheetView tabSelected="1" topLeftCell="GF20" zoomScale="57" zoomScaleNormal="32" workbookViewId="0">
+      <selection activeCell="GV8" sqref="GV8:GV29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.41796875" defaultRowHeight="49" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3072,11 +3071,11 @@
     <col min="7" max="7" width="7.41796875" style="2" customWidth="1"/>
     <col min="8" max="13" width="8.41796875" style="2" customWidth="1"/>
     <col min="14" max="14" width="8.41796875" style="6" customWidth="1"/>
-    <col min="15" max="308" width="8.41796875" style="2" customWidth="1"/>
-    <col min="309" max="16384" width="20.41796875" style="2"/>
+    <col min="15" max="309" width="8.41796875" style="2" customWidth="1"/>
+    <col min="310" max="16384" width="20.41796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:201" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:204" s="1" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -3265,7 +3264,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="2" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>90</v>
       </c>
@@ -3456,7 +3455,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>175</v>
       </c>
@@ -3633,7 +3632,7 @@
         <v>8.0043000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4" t="s">
         <v>180</v>
       </c>
@@ -3784,7 +3783,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="5" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="S5" s="2" t="s">
         <v>207</v>
       </c>
@@ -3810,7 +3809,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>209</v>
       </c>
@@ -3917,7 +3916,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="O7" s="2">
         <v>0.1</v>
       </c>
@@ -4367,10 +4366,13 @@
         <v>385</v>
       </c>
       <c r="GS7" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="GT7" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4" t="s">
         <v>251</v>
       </c>
@@ -4646,7 +4648,7 @@
         <v>0.1</v>
       </c>
       <c r="DL8" s="2">
-        <f t="shared" ref="DL8:DL23" si="21">$CB$3*DK8/(1+$CB$3*DK8)</f>
+        <f>$CB$3*DK8/(1+$CB$3*DK8)</f>
         <v>1.6145059572416642E-2</v>
       </c>
       <c r="DM8" s="2">
@@ -4663,7 +4665,7 @@
         <v>0.91900000000000004</v>
       </c>
       <c r="DR8">
-        <f t="shared" ref="DR8:DR32" si="22">EXP(-2*DO8*DQ8/55.51)</f>
+        <f t="shared" ref="DR8:DR32" si="21">EXP(-2*DO8*DQ8/55.51)</f>
         <v>0.9933996484160329</v>
       </c>
       <c r="DS8"/>
@@ -4671,98 +4673,98 @@
         <v>0.2</v>
       </c>
       <c r="DU8" s="2">
-        <f t="shared" ref="DU8:DU32" si="23">$CD$3*DT8/(1+$CD$3*DT8)</f>
+        <f t="shared" ref="DU8:DU32" si="22">$CD$3*DT8/(1+$CD$3*DT8)</f>
         <v>2.3902671383168955E-2</v>
       </c>
       <c r="DV8" s="2">
         <v>0.95750000000000002</v>
       </c>
       <c r="DW8">
-        <f t="shared" ref="DW8:DW32" si="24">EXP(-2*DT8*DV8/55.51)</f>
+        <f t="shared" ref="DW8:DW32" si="23">EXP(-2*DT8*DV8/55.51)</f>
         <v>0.99312409026993709</v>
       </c>
       <c r="DY8" s="2">
         <v>0.2</v>
       </c>
       <c r="DZ8" s="2">
-        <f t="shared" ref="DZ8:DZ13" si="25">$CE$3*DY8/(1+$CE$3*DY8)</f>
+        <f t="shared" ref="DZ8:DZ13" si="24">$CE$3*DY8/(1+$CE$3*DY8)</f>
         <v>2.3923631784950855E-2</v>
       </c>
       <c r="EA8" s="2">
         <v>0.88759999999999994</v>
       </c>
       <c r="EB8">
-        <f t="shared" ref="EB8:EB13" si="26">EXP(-2*DY8*EA8/55.51)</f>
+        <f t="shared" ref="EB8:EB13" si="25">EXP(-2*DY8*EA8/55.51)</f>
         <v>0.99362444595268207</v>
       </c>
       <c r="ED8" s="2">
         <v>2.0030000000000001</v>
       </c>
       <c r="EE8" s="2">
-        <f t="shared" ref="EE8:EE13" si="27">$CF$3*ED8/(1+$CF$3*ED8)</f>
+        <f t="shared" ref="EE8:EE13" si="26">$CF$3*ED8/(1+$CF$3*ED8)</f>
         <v>0.17087356437897722</v>
       </c>
       <c r="EF8" s="2">
         <v>1.02</v>
       </c>
       <c r="EG8">
-        <f t="shared" ref="EG8:EG13" si="28">EXP(-2*ED8*EF8/55.51)</f>
+        <f t="shared" ref="EG8:EG13" si="27">EXP(-2*ED8*EF8/55.51)</f>
         <v>0.92903346275659915</v>
       </c>
       <c r="EI8" s="2">
         <v>1.004</v>
       </c>
       <c r="EJ8" s="2">
-        <f t="shared" ref="EJ8:EJ15" si="29">$CG$3*EI8/(1+$CG$3*EI8)</f>
+        <f t="shared" ref="EJ8:EJ15" si="28">$CG$3*EI8/(1+$CG$3*EI8)</f>
         <v>0.13080480278326037</v>
       </c>
       <c r="EK8" s="2">
         <v>0.93</v>
       </c>
       <c r="EL8">
-        <f t="shared" ref="EL8:EL15" si="30">EXP(-2*EI8*EK8/55.51)</f>
+        <f t="shared" ref="EL8:EL15" si="29">EXP(-2*EI8*EK8/55.51)</f>
         <v>0.96691807680701369</v>
       </c>
       <c r="EN8" s="2">
         <v>1.2549999999999999</v>
       </c>
       <c r="EO8" s="2">
-        <f t="shared" ref="EO8:EO13" si="31">$CH$3*EN8/(1+$CH$3*EN8)</f>
+        <f t="shared" ref="EO8:EO13" si="30">$CH$3*EN8/(1+$CH$3*EN8)</f>
         <v>0.12993922625495388</v>
       </c>
       <c r="EP8" s="2">
         <v>1.07</v>
       </c>
       <c r="EQ8">
-        <f t="shared" ref="EQ8:EQ13" si="32">EXP(-2*EN8*EP8/55.51)</f>
+        <f t="shared" ref="EQ8:EQ13" si="31">EXP(-2*EN8*EP8/55.51)</f>
         <v>0.95276949895611107</v>
       </c>
       <c r="ES8" s="2">
         <v>1.4930000000000001</v>
       </c>
       <c r="ET8" s="2">
-        <f t="shared" ref="ET8:ET13" si="33">$CI$3*ES8/(1+$CI$3*ES8)</f>
+        <f t="shared" ref="ET8:ET13" si="32">$CI$3*ES8/(1+$CI$3*ES8)</f>
         <v>0.15292539417515585</v>
       </c>
       <c r="EU8" s="2">
         <v>0.9</v>
       </c>
       <c r="EV8">
-        <f t="shared" ref="EV8:EV13" si="34">EXP(-2*ES8*EU8/55.51)</f>
+        <f t="shared" ref="EV8:EV13" si="33">EXP(-2*ES8*EU8/55.51)</f>
         <v>0.95274032072972648</v>
       </c>
       <c r="EX8" s="2">
         <v>1.57</v>
       </c>
       <c r="EY8" s="2">
-        <f t="shared" ref="EY8:EY13" si="35">$CJ$3*EX8/(1+$CJ$3*EX8)</f>
+        <f t="shared" ref="EY8:EY13" si="34">$CJ$3*EX8/(1+$CJ$3*EX8)</f>
         <v>0.25043757580418491</v>
       </c>
       <c r="EZ8" s="2">
         <v>0.94</v>
       </c>
       <c r="FA8">
-        <f t="shared" ref="FA8:FA13" si="36">EXP(-2*EX8*EZ8/55.51)</f>
+        <f t="shared" ref="FA8:FA13" si="35">EXP(-2*EX8*EZ8/55.51)</f>
         <v>0.9482165245628732</v>
       </c>
       <c r="FC8" s="2">
@@ -4783,15 +4785,15 @@
         <v>1.006</v>
       </c>
       <c r="FI8" s="2">
-        <f t="shared" ref="FI8:FI15" si="37">$CL$3*FH8/(1+$CL$3*FH8)</f>
+        <f t="shared" ref="FI8:FI15" si="36">$CL$3*FH8/(1+$CL$3*FH8)</f>
         <v>0.16742246667512675</v>
       </c>
       <c r="FJ8" s="2">
         <v>1.3</v>
       </c>
       <c r="FK8">
-        <f t="shared" ref="FK8:FK15" si="38">EXP(-2*FH8*FJ8/55.51)</f>
-        <v>0.95397345016283042</v>
+        <f>EXP(-3*FH8*FJ8/55.51)</f>
+        <v>0.93176079318812899</v>
       </c>
       <c r="FM8" s="2">
         <v>1.1379999999999999</v>
@@ -4804,50 +4806,50 @@
         <v>1.19</v>
       </c>
       <c r="FP8">
-        <f>EXP(-2*FM8*FO8/55.51)</f>
-        <v>0.95237927122752064</v>
+        <f>EXP(-3*FM8*FO8/55.51)</f>
+        <v>0.92942617994781596</v>
       </c>
       <c r="FR8" s="2">
         <v>0.66200000000000003</v>
       </c>
       <c r="FS8" s="2">
-        <f t="shared" ref="FS8:FS15" si="39">$CN$3*FR8/(1+$CN$3*FR8)</f>
+        <f t="shared" ref="FS8:FS15" si="37">$CN$3*FR8/(1+$CN$3*FR8)</f>
         <v>9.4979101528918766E-2</v>
       </c>
       <c r="FT8" s="2">
         <v>0.94</v>
       </c>
       <c r="FU8">
-        <f t="shared" ref="FU8:FU15" si="40">EXP(-2*FR8*FT8/55.51)</f>
-        <v>0.97782900594463251</v>
+        <f>EXP(-3*FR8*FT8/55.51)</f>
+        <v>0.96692852814878061</v>
       </c>
       <c r="FW8" s="2">
         <v>0.8</v>
       </c>
       <c r="FX8" s="2">
-        <f t="shared" ref="FX8:FX15" si="41">$CO$3*FW8/(1+$CO$3*FW8)</f>
+        <f t="shared" ref="FX8:FX15" si="38">$CO$3*FW8/(1+$CO$3*FW8)</f>
         <v>0.16523643843117874</v>
       </c>
       <c r="FY8" s="2">
         <v>1.52</v>
       </c>
       <c r="FZ8">
-        <f t="shared" ref="FZ8:FZ15" si="42">EXP(-2*FW8*FY8/55.51)</f>
-        <v>0.95713395276870528</v>
+        <f>EXP(-3*FW8*FY8/55.51)</f>
+        <v>0.93639499467134213</v>
       </c>
       <c r="GB8" s="2">
         <v>0.97</v>
       </c>
       <c r="GC8" s="2">
-        <f t="shared" ref="GC8:GC15" si="43">$CP$3*GB8/(1+$CP$3*GB8)</f>
+        <f t="shared" ref="GC8:GC15" si="39">$CP$3*GB8/(1+$CP$3*GB8)</f>
         <v>0.24879079732668685</v>
       </c>
       <c r="GD8" s="2">
         <v>1.26</v>
       </c>
       <c r="GE8">
-        <f t="shared" ref="GE8:GE15" si="44">EXP(-2*GB8*GD8/55.51)</f>
-        <v>0.95692016902693289</v>
+        <f>EXP(-3*GB8*GD8/55.51)</f>
+        <v>0.93608128490306408</v>
       </c>
       <c r="GG8" s="2">
         <v>0.504</v>
@@ -4860,35 +4862,47 @@
         <v>1.5</v>
       </c>
       <c r="GJ8">
-        <f>EXP(-2*GG8*GI8/55.51)</f>
-        <v>0.97312928269247323</v>
+        <f>EXP(-3*GG8*GI8/55.51)</f>
+        <v>0.9599659123181703</v>
       </c>
       <c r="GL8" s="2">
         <v>1.0009999999999999</v>
       </c>
       <c r="GM8" s="2">
-        <f t="shared" ref="GM8:GM15" si="45">$CR$3*GL8/(1+$CR$3*GL8)</f>
+        <f t="shared" ref="GM8:GM15" si="40">$CR$3*GL8/(1+$CR$3*GL8)</f>
         <v>0.22924975001101011</v>
       </c>
       <c r="GN8" s="2">
         <v>1.17</v>
       </c>
       <c r="GO8">
-        <f t="shared" ref="GO8:GO15" si="46">EXP(-2*GL8*GN8/55.51)</f>
-        <v>0.95868116900428202</v>
+        <f>EXP(-3*GL8*GN8/55.51)</f>
+        <v>0.93866644927627962</v>
       </c>
       <c r="GQ8" s="2">
-        <f>(1/GR8)/BH3</f>
-        <v>15.002512920914251</v>
+        <f>(1/GR8)/$BH$3</f>
+        <v>1.8140293401105472</v>
       </c>
       <c r="GR8" s="2">
-        <v>3.7</v>
+        <v>30.6</v>
       </c>
       <c r="GS8" s="2">
-        <v>0.73199999999999998</v>
+        <f>$CS$3*GQ8/(1+$CS$3*GQ8)</f>
+        <v>0.12679034756740831</v>
+      </c>
+      <c r="GT8" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="GU8" s="2">
+        <f>1-(GQ8/(55.51))/(GQ8/(55.51) +1)</f>
+        <v>0.96835481802321177</v>
+      </c>
+      <c r="GV8" s="2">
+        <f>GT8/GU8</f>
+        <v>0.98104535891019662</v>
       </c>
     </row>
-    <row r="9" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4" t="s">
         <v>258</v>
       </c>
@@ -5108,7 +5122,7 @@
         <v>0.3</v>
       </c>
       <c r="CR9" s="2">
-        <f t="shared" ref="CR9:CR18" si="47">$BW$3*CQ9/(1+$BW$3*CQ9)</f>
+        <f t="shared" ref="CR9:CR18" si="41">$BW$3*CQ9/(1+$BW$3*CQ9)</f>
         <v>4.5694604446998244E-2</v>
       </c>
       <c r="CS9" s="2">
@@ -5158,7 +5172,7 @@
         <v>0.2</v>
       </c>
       <c r="DL9" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="DL9:DL23" si="42">$CB$3*DK9/(1+$CB$3*DK9)</f>
         <v>3.1777076354059755E-2</v>
       </c>
       <c r="DM9" s="2">
@@ -5175,105 +5189,105 @@
         <v>0.91420000000000001</v>
       </c>
       <c r="DR9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.99016719844072409</v>
       </c>
       <c r="DT9" s="2">
         <v>0.3</v>
       </c>
       <c r="DU9" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>3.5430564504616423E-2</v>
       </c>
       <c r="DV9" s="2">
         <v>0.97099999999999997</v>
       </c>
       <c r="DW9">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.98955947836302427</v>
       </c>
       <c r="DY9" s="2">
         <v>0.3</v>
       </c>
       <c r="DZ9" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>3.5461266535810915E-2</v>
       </c>
       <c r="EA9" s="2">
         <v>0.86770000000000003</v>
       </c>
       <c r="EB9">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0.99066499358569005</v>
       </c>
       <c r="ED9" s="2">
         <v>2.9940000000000002</v>
       </c>
       <c r="EE9" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0.23550478464681998</v>
       </c>
       <c r="EF9" s="2">
         <v>1.19</v>
       </c>
       <c r="EG9">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>0.87952945746590139</v>
       </c>
       <c r="EI9" s="2">
         <v>1.673</v>
       </c>
       <c r="EJ9" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.20048992058842152</v>
       </c>
       <c r="EK9" s="2">
         <v>1.01</v>
       </c>
       <c r="EL9">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.94093595549059772</v>
       </c>
       <c r="EN9" s="2">
         <v>1.6080000000000001</v>
       </c>
       <c r="EO9" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0.16061751690516321</v>
       </c>
       <c r="EP9" s="2">
         <v>0.96</v>
       </c>
       <c r="EQ9">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0.94590031870385338</v>
       </c>
       <c r="ES9" s="2">
         <v>2.968</v>
       </c>
       <c r="ET9" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.26410556564614002</v>
       </c>
       <c r="EU9" s="2">
         <v>0.95</v>
       </c>
       <c r="EV9">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>0.90340086081526783</v>
       </c>
       <c r="EX9" s="2">
         <v>2.2440000000000002</v>
       </c>
       <c r="EY9" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.32320195537242424</v>
       </c>
       <c r="EZ9" s="2">
         <v>0.88</v>
       </c>
       <c r="FA9">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.93132380235784307</v>
       </c>
       <c r="FC9" s="2">
@@ -5294,15 +5308,15 @@
         <v>1.238</v>
       </c>
       <c r="FI9" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.19837354481350811</v>
       </c>
       <c r="FJ9" s="2">
         <v>1.37</v>
       </c>
       <c r="FK9">
-        <f t="shared" si="38"/>
-        <v>0.94072138350529388</v>
+        <f t="shared" ref="FK9:FK15" si="43">EXP(-3*FH9*FJ9/55.51)</f>
+        <v>0.91241312533455632</v>
       </c>
       <c r="FM9" s="2">
         <v>1.464</v>
@@ -5315,50 +5329,50 @@
         <v>1.25</v>
       </c>
       <c r="FP9">
-        <f>EXP(-2*FM9*FO9/55.51)</f>
-        <v>0.93619258924061399</v>
+        <f t="shared" ref="FP9:FP12" si="44">EXP(-3*FM9*FO9/55.51)</f>
+        <v>0.90583229140256794</v>
       </c>
       <c r="FR9" s="2">
         <v>0.871</v>
       </c>
       <c r="FS9" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>0.12132686181194545</v>
       </c>
       <c r="FT9" s="2">
         <v>0.82</v>
       </c>
       <c r="FU9">
-        <f t="shared" si="40"/>
-        <v>0.97459525126863267</v>
+        <f t="shared" ref="FU9:FU15" si="45">EXP(-3*FR9*FT9/55.51)</f>
+        <v>0.96213593702938704</v>
       </c>
       <c r="FW9" s="2">
         <v>1.0129999999999999</v>
       </c>
       <c r="FX9" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>0.20041360365441047</v>
       </c>
       <c r="FY9" s="2">
         <v>1.29</v>
       </c>
       <c r="FZ9">
-        <f t="shared" si="42"/>
-        <v>0.95400885318520878</v>
+        <f t="shared" ref="FZ9:FZ15" si="46">EXP(-3*FW9*FY9/55.51)</f>
+        <v>0.9318126616980742</v>
       </c>
       <c r="GB9" s="2">
         <v>1.264</v>
       </c>
       <c r="GC9" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="39"/>
         <v>0.3014650122824804</v>
       </c>
       <c r="GD9" s="2">
         <v>1.37</v>
       </c>
       <c r="GE9">
-        <f t="shared" si="44"/>
-        <v>0.93951486205196444</v>
+        <f t="shared" ref="GE9:GE15" si="47">EXP(-3*GB9*GD9/55.51)</f>
+        <v>0.91065836619725982</v>
       </c>
       <c r="GG9" s="2">
         <v>0.73799999999999999</v>
@@ -5371,35 +5385,47 @@
         <v>1.27</v>
       </c>
       <c r="GJ9">
-        <f>EXP(-2*GG9*GI9/55.51)</f>
-        <v>0.96679475950506333</v>
+        <f t="shared" ref="GJ9:GJ12" si="48">EXP(-3*GG9*GI9/55.51)</f>
+        <v>0.95060792696283825</v>
       </c>
       <c r="GL9" s="2">
         <v>1.2649999999999999</v>
       </c>
       <c r="GM9" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0.27319353889406656</v>
       </c>
       <c r="GN9" s="2">
         <v>1.19</v>
       </c>
       <c r="GO9">
-        <f t="shared" si="46"/>
-        <v>0.94720752122541474</v>
+        <f t="shared" ref="GO9:GO15" si="49">EXP(-3*GL9*GN9/55.51)</f>
+        <v>0.92186580697230458</v>
       </c>
       <c r="GQ9" s="2">
-        <f>(1/GR9)/BH3</f>
-        <v>16.326264060994923</v>
+        <f t="shared" ref="GQ9:GQ29" si="50">(1/GR9)/$BH$3</f>
+        <v>2.6432998955896538</v>
       </c>
       <c r="GR9" s="2">
-        <v>3.4</v>
+        <v>21</v>
       </c>
       <c r="GS9" s="2">
-        <v>0.71499999999999997</v>
+        <f t="shared" ref="GS9:GS29" si="51">$CS$3*GQ9/(1+$CS$3*GQ9)</f>
+        <v>0.17462987446493788</v>
+      </c>
+      <c r="GT9" s="2">
+        <v>0.93</v>
+      </c>
+      <c r="GU9" s="2">
+        <f t="shared" ref="GU9:GU28" si="52">1-(GQ9/(55.51))/(GQ9/(55.51) +1)</f>
+        <v>0.95454600340246343</v>
+      </c>
+      <c r="GV9" s="2">
+        <f t="shared" ref="GV9:GV29" si="53">GT9/GU9</f>
+        <v>0.97428515407851524</v>
       </c>
     </row>
-    <row r="10" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="O10" s="2">
         <v>3</v>
       </c>
@@ -5610,7 +5636,7 @@
         <v>0.4</v>
       </c>
       <c r="CR10" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="41"/>
         <v>6.001206342918277E-2</v>
       </c>
       <c r="CS10" s="2">
@@ -5660,7 +5686,7 @@
         <v>0.3</v>
       </c>
       <c r="DL10" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>4.6920122375456279E-2</v>
       </c>
       <c r="DM10" s="2">
@@ -5677,105 +5703,105 @@
         <v>0.91149999999999998</v>
       </c>
       <c r="DR10">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.98694953373358874</v>
       </c>
       <c r="DT10" s="2">
         <v>0.4</v>
       </c>
       <c r="DU10" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>4.668934274950047E-2</v>
       </c>
       <c r="DV10" s="2">
         <v>0.98550000000000004</v>
       </c>
       <c r="DW10">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.98589753827697413</v>
       </c>
       <c r="DY10" s="2">
         <v>0.4</v>
       </c>
       <c r="DZ10" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>4.6729328325484737E-2</v>
       </c>
       <c r="EA10" s="2">
         <v>0.84989999999999999</v>
       </c>
       <c r="EB10">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0.98782610495573842</v>
       </c>
       <c r="ED10" s="2">
         <v>4.0119999999999996</v>
       </c>
       <c r="EE10" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0.29218306512875597</v>
       </c>
       <c r="EF10" s="2">
         <v>1.23</v>
       </c>
       <c r="EG10">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>0.83711221141098335</v>
       </c>
       <c r="EI10" s="2">
         <v>2.1579999999999999</v>
       </c>
       <c r="EJ10" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.24440631349300973</v>
       </c>
       <c r="EK10" s="2">
         <v>1.1100000000000001</v>
       </c>
       <c r="EL10">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.91731491250019648</v>
       </c>
       <c r="EN10" s="2">
         <v>2.2200000000000002</v>
       </c>
       <c r="EO10" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0.20897340568589917</v>
       </c>
       <c r="EP10" s="2">
         <v>0.95</v>
       </c>
       <c r="EQ10">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0.92682889589713979</v>
       </c>
       <c r="ES10" s="2">
         <v>3.55</v>
       </c>
       <c r="ET10" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.30034017460710605</v>
       </c>
       <c r="EU10" s="2">
         <v>0.98</v>
       </c>
       <c r="EV10">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>0.88219091951636441</v>
       </c>
       <c r="EX10" s="2">
         <v>2.7679999999999998</v>
       </c>
       <c r="EY10" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.37069638134309096</v>
       </c>
       <c r="EZ10" s="2">
         <v>0.81</v>
       </c>
       <c r="FA10">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.92239556281327817</v>
       </c>
       <c r="FC10" s="2">
@@ -5796,15 +5822,15 @@
         <v>1.7090000000000001</v>
       </c>
       <c r="FI10" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.25462802021278863</v>
       </c>
       <c r="FJ10" s="2">
         <v>1.47</v>
       </c>
       <c r="FK10">
-        <f t="shared" si="38"/>
-        <v>0.91346108689128158</v>
+        <f t="shared" si="43"/>
+        <v>0.87304187908091491</v>
       </c>
       <c r="FM10" s="2">
         <v>1.875</v>
@@ -5817,50 +5843,50 @@
         <v>1.37</v>
       </c>
       <c r="FP10">
-        <f>EXP(-2*FM10*FO10/55.51)</f>
-        <v>0.91160281673840204</v>
+        <f t="shared" si="44"/>
+        <v>0.87037916747218236</v>
       </c>
       <c r="FR10" s="2">
         <v>1.2989999999999999</v>
       </c>
       <c r="FS10" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>0.17076479541975584</v>
       </c>
       <c r="FT10" s="2">
         <v>1.1200000000000001</v>
       </c>
       <c r="FU10">
-        <f t="shared" si="40"/>
-        <v>0.94893150087008038</v>
+        <f t="shared" si="45"/>
+        <v>0.92438373590379708</v>
       </c>
       <c r="FW10" s="2">
         <v>1.345</v>
       </c>
       <c r="FX10" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>0.24969613631400547</v>
       </c>
       <c r="FY10" s="2">
         <v>1.22</v>
       </c>
       <c r="FZ10">
-        <f t="shared" si="42"/>
-        <v>0.94259282247862319</v>
+        <f t="shared" si="46"/>
+        <v>0.91513716422800773</v>
       </c>
       <c r="GB10" s="2">
         <v>1.534</v>
       </c>
       <c r="GC10" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="39"/>
         <v>0.34372592335498442</v>
       </c>
       <c r="GD10" s="2">
         <v>1.42</v>
       </c>
       <c r="GE10">
-        <f t="shared" si="44"/>
-        <v>0.92451829840074184</v>
+        <f t="shared" si="47"/>
+        <v>0.88894167468778684</v>
       </c>
       <c r="GG10" s="2">
         <v>0.97499999999999998</v>
@@ -5873,35 +5899,47 @@
         <v>1.2</v>
       </c>
       <c r="GJ10">
-        <f>EXP(-2*GG10*GI10/55.51)</f>
-        <v>0.95872158264541152</v>
+        <f t="shared" si="48"/>
+        <v>0.93872580476906919</v>
       </c>
       <c r="GL10" s="2">
         <v>1.4450000000000001</v>
       </c>
       <c r="GM10" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0.30038975986088384</v>
       </c>
       <c r="GN10" s="2">
         <v>1.24</v>
       </c>
       <c r="GO10">
-        <f t="shared" si="46"/>
-        <v>0.93748198497898005</v>
+        <f t="shared" si="49"/>
+        <v>0.907704307439411</v>
       </c>
       <c r="GQ10" s="2">
-        <f>(1/GR10)/BH3</f>
-        <v>17.346655564807104</v>
+        <f t="shared" si="50"/>
+        <v>3.5812450198311443</v>
       </c>
       <c r="GR10" s="2">
-        <v>3.2</v>
+        <v>15.5</v>
       </c>
       <c r="GS10" s="2">
-        <v>0.70599999999999996</v>
+        <f t="shared" si="51"/>
+        <v>0.22279003160527228</v>
+      </c>
+      <c r="GT10" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="GU10" s="2">
+        <f t="shared" si="52"/>
+        <v>0.93939465958740132</v>
+      </c>
+      <c r="GV10" s="2">
+        <f t="shared" si="53"/>
+        <v>0.96870893475133024</v>
       </c>
     </row>
-    <row r="11" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4" t="s">
         <v>267</v>
       </c>
@@ -6124,7 +6162,7 @@
         <v>0.5</v>
       </c>
       <c r="CR11" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="41"/>
         <v>7.3906262458854816E-2</v>
       </c>
       <c r="CS11" s="2">
@@ -6174,7 +6212,7 @@
         <v>0.4</v>
       </c>
       <c r="DL11" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>6.1596786907398379E-2</v>
       </c>
       <c r="DM11" s="2">
@@ -6191,105 +6229,105 @@
         <v>0.91020000000000001</v>
       </c>
       <c r="DR11">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.98373665421648882</v>
       </c>
       <c r="DT11" s="2">
         <v>0.5</v>
       </c>
       <c r="DU11" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>5.7688320989050329E-2</v>
       </c>
       <c r="DV11" s="2">
         <v>0.99950000000000006</v>
       </c>
       <c r="DW11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.98215537048432389</v>
       </c>
       <c r="DY11" s="2">
         <v>0.5</v>
       </c>
       <c r="DZ11" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>5.7737155779604719E-2</v>
       </c>
       <c r="EA11" s="2">
         <v>0.83330000000000004</v>
       </c>
       <c r="EB11">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0.98510040440198543</v>
       </c>
       <c r="ED11" s="2">
         <v>4.9889999999999999</v>
       </c>
       <c r="EE11" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0.33920044482911493</v>
       </c>
       <c r="EF11" s="2">
         <v>1.26</v>
       </c>
       <c r="EG11">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>0.79732989957467659</v>
       </c>
       <c r="EI11" s="2">
         <v>3.3029999999999999</v>
       </c>
       <c r="EJ11" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.33114245477153503</v>
       </c>
       <c r="EK11" s="2">
         <v>1.26</v>
       </c>
       <c r="EL11">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.86075356367894651</v>
       </c>
       <c r="EN11" s="2">
         <v>3.0209999999999999</v>
       </c>
       <c r="EO11" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0.26443491315550799</v>
       </c>
       <c r="EP11" s="2">
         <v>0.96</v>
       </c>
       <c r="EQ11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0.90078250538489457</v>
       </c>
       <c r="ES11" s="2">
         <v>4.4630000000000001</v>
       </c>
       <c r="ET11" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.35050847003203212</v>
       </c>
       <c r="EU11" s="2">
         <v>0.98</v>
       </c>
       <c r="EV11">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>0.85420517801429519</v>
       </c>
       <c r="EX11" s="2">
         <v>3.4849999999999999</v>
       </c>
       <c r="EY11" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.42582946899819329</v>
       </c>
       <c r="EZ11" s="2">
         <v>0.81</v>
       </c>
       <c r="FA11">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.90329508236438283</v>
       </c>
       <c r="FC11" s="2">
@@ -6310,15 +6348,15 @@
         <v>2.254</v>
       </c>
       <c r="FI11" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.31060730078174514</v>
       </c>
       <c r="FJ11" s="2">
         <v>1.71</v>
       </c>
       <c r="FK11">
-        <f t="shared" si="38"/>
-        <v>0.87034106667801636</v>
+        <f t="shared" si="43"/>
+        <v>0.81195921311206065</v>
       </c>
       <c r="FM11" s="2">
         <v>2.2730000000000001</v>
@@ -6331,50 +6369,50 @@
         <v>1.38</v>
       </c>
       <c r="FP11">
-        <f>EXP(-2*FM11*FO11/55.51)</f>
-        <v>0.89313698380096151</v>
+        <f t="shared" si="44"/>
+        <v>0.8440673670140969</v>
       </c>
       <c r="FR11" s="2">
         <v>1.5029999999999999</v>
       </c>
       <c r="FS11" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>0.192422069880542</v>
       </c>
       <c r="FT11" s="2">
         <v>1.31</v>
       </c>
       <c r="FU11">
-        <f t="shared" si="40"/>
-        <v>0.93151810707080429</v>
+        <f t="shared" si="45"/>
+        <v>0.89905643086863507</v>
       </c>
       <c r="FW11" s="2">
         <v>1.746</v>
       </c>
       <c r="FX11" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>0.3016822098473172</v>
       </c>
       <c r="FY11" s="2">
         <v>1.36</v>
       </c>
       <c r="FZ11">
-        <f t="shared" si="42"/>
-        <v>0.91800328077604243</v>
+        <f t="shared" si="46"/>
+        <v>0.87956178088623849</v>
       </c>
       <c r="GB11" s="2">
         <v>1.96</v>
       </c>
       <c r="GC11" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="39"/>
         <v>0.40091162080485371</v>
       </c>
       <c r="GD11" s="2">
         <v>1.6</v>
       </c>
       <c r="GE11">
-        <f t="shared" si="44"/>
-        <v>0.89316079681406857</v>
+        <f t="shared" si="47"/>
+        <v>0.84410112430152451</v>
       </c>
       <c r="GG11" s="2">
         <v>1.214</v>
@@ -6387,35 +6425,47 @@
         <v>1.27</v>
       </c>
       <c r="GJ11">
-        <f>EXP(-2*GG11*GI11/55.51)</f>
-        <v>0.94596507359925908</v>
+        <f t="shared" si="48"/>
+        <v>0.92005259136495299</v>
       </c>
       <c r="GL11" s="2">
         <v>1.706</v>
       </c>
       <c r="GM11" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0.33639513539410604</v>
       </c>
       <c r="GN11" s="2">
         <v>1.3</v>
       </c>
       <c r="GO11">
-        <f t="shared" si="46"/>
-        <v>0.92320282503628792</v>
+        <f t="shared" si="49"/>
+        <v>0.88704507129596977</v>
       </c>
       <c r="GQ11" s="2">
-        <f>(1/GR10)/BH3</f>
-        <v>17.346655564807104</v>
+        <f t="shared" si="50"/>
+        <v>4.6257748172818944</v>
       </c>
       <c r="GR11" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="GS11" s="2">
-        <v>0.69699999999999995</v>
+        <f t="shared" si="51"/>
+        <v>0.27021196868575359</v>
+      </c>
+      <c r="GT11" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="GU11" s="2">
+        <f t="shared" si="52"/>
+        <v>0.92307782129128679</v>
+      </c>
+      <c r="GV11" s="2">
+        <f t="shared" si="53"/>
+        <v>0.96416572847020154</v>
       </c>
     </row>
-    <row r="12" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4" t="s">
         <v>275</v>
       </c>
@@ -6635,7 +6685,7 @@
         <v>0.6</v>
       </c>
       <c r="CR12" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="41"/>
         <v>8.7395697085313417E-2</v>
       </c>
       <c r="CS12" s="2">
@@ -6675,7 +6725,7 @@
         <v>0.5</v>
       </c>
       <c r="DL12" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>7.5828288896076887E-2</v>
       </c>
       <c r="DM12" s="2">
@@ -6692,105 +6742,105 @@
         <v>0.90959999999999996</v>
       </c>
       <c r="DR12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.98052858129423781</v>
       </c>
       <c r="DT12" s="2">
         <v>0.6</v>
       </c>
       <c r="DU12" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>6.8436389110394E-2</v>
       </c>
       <c r="DV12" s="2">
         <v>1.0135000000000001</v>
       </c>
       <c r="DW12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.97832870538154948</v>
       </c>
       <c r="DY12" s="2">
         <v>0.6</v>
       </c>
       <c r="DZ12" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>6.8493661099363778E-2</v>
       </c>
       <c r="EA12" s="2">
         <v>0.81730000000000003</v>
       </c>
       <c r="EB12">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0.98248699899859548</v>
       </c>
       <c r="ED12" s="2">
         <v>5.8010000000000002</v>
       </c>
       <c r="EE12" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0.37377294330768335</v>
       </c>
       <c r="EF12" s="2">
         <v>1.35</v>
       </c>
       <c r="EG12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>0.75415303213518359</v>
       </c>
       <c r="EI12" s="2">
         <v>3.9580000000000002</v>
       </c>
       <c r="EJ12" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.372357869843366</v>
       </c>
       <c r="EK12" s="2">
         <v>1.34</v>
       </c>
       <c r="EL12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.82605773211349576</v>
       </c>
       <c r="EN12" s="2">
         <v>3.81</v>
       </c>
       <c r="EO12" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0.31195343300834599</v>
       </c>
       <c r="EP12" s="2">
         <v>0.97</v>
       </c>
       <c r="EQ12">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0.87532994246531504</v>
       </c>
       <c r="ES12" s="2">
         <v>5.9960000000000004</v>
       </c>
       <c r="ET12" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.42030206065458381</v>
       </c>
       <c r="EU12" s="2">
         <v>1.07</v>
       </c>
       <c r="EV12">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>0.7936160749499328</v>
       </c>
       <c r="EX12" s="2">
         <v>4.32</v>
       </c>
       <c r="EY12" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.47898735148013444</v>
       </c>
       <c r="EZ12" s="2">
         <v>0.79</v>
       </c>
       <c r="FA12">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.88429759370363636</v>
       </c>
       <c r="FC12" s="2">
@@ -6811,15 +6861,15 @@
         <v>3.0219999999999998</v>
       </c>
       <c r="FI12" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.37658486932327373</v>
       </c>
       <c r="FJ12" s="2">
         <v>2.06</v>
       </c>
       <c r="FK12">
-        <f t="shared" si="38"/>
-        <v>0.79907901777861967</v>
+        <f t="shared" si="43"/>
+        <v>0.71430648117847162</v>
       </c>
       <c r="FM12" s="2">
         <v>2.915</v>
@@ -6832,50 +6882,50 @@
         <v>1.75</v>
       </c>
       <c r="FP12">
-        <f>EXP(-2*FM12*FO12/55.51)</f>
-        <v>0.83210577528624219</v>
+        <f t="shared" si="44"/>
+        <v>0.75904549040402636</v>
       </c>
       <c r="FR12" s="2">
         <v>1.7969999999999999</v>
       </c>
       <c r="FS12" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>0.22171624006041163</v>
       </c>
       <c r="FT12" s="2">
         <v>1.35</v>
       </c>
       <c r="FU12">
-        <f t="shared" si="40"/>
-        <v>0.9163051168124039</v>
+        <f t="shared" si="45"/>
+        <v>0.87712233019881447</v>
       </c>
       <c r="FW12" s="2">
         <v>1.996</v>
       </c>
       <c r="FX12" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>0.33059783477317722</v>
       </c>
       <c r="FY12" s="2">
         <v>1.54</v>
       </c>
       <c r="FZ12">
-        <f t="shared" si="42"/>
-        <v>0.89516335820863435</v>
+        <f t="shared" si="46"/>
+        <v>0.84694156155146061</v>
       </c>
       <c r="GB12" s="2">
         <v>2.37</v>
       </c>
       <c r="GC12" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="39"/>
         <v>0.44726618129636092</v>
       </c>
       <c r="GD12" s="2">
         <v>1.79</v>
       </c>
       <c r="GE12">
-        <f t="shared" si="44"/>
-        <v>0.85826005117329662</v>
+        <f t="shared" si="47"/>
+        <v>0.79511207199004585</v>
       </c>
       <c r="GG12" s="2">
         <v>1.3879999999999999</v>
@@ -6888,35 +6938,47 @@
         <v>1.29</v>
       </c>
       <c r="GJ12">
-        <f>EXP(-2*GG12*GI12/55.51)</f>
-        <v>0.93752522059819665</v>
+        <f t="shared" si="48"/>
+        <v>0.90776710162251328</v>
       </c>
       <c r="GL12" s="2">
         <v>1.8879999999999999</v>
       </c>
       <c r="GM12" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0.35938514093321899</v>
       </c>
       <c r="GN12" s="2">
         <v>1.34</v>
       </c>
       <c r="GO12">
-        <f t="shared" si="46"/>
-        <v>0.91287906642256578</v>
+        <f t="shared" si="49"/>
+        <v>0.87220761153081561</v>
       </c>
       <c r="GQ12" s="2">
-        <f>(1/GR11)/BH3</f>
-        <v>18.503099269127578</v>
+        <f t="shared" si="50"/>
+        <v>5.7226080213796644</v>
       </c>
       <c r="GR12" s="2">
-        <v>2.9</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="GS12" s="2">
-        <v>0.68600000000000005</v>
+        <f t="shared" si="51"/>
+        <v>0.31415468123561313</v>
+      </c>
+      <c r="GT12" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="GU12" s="2">
+        <f t="shared" si="52"/>
+        <v>0.90654312781546742</v>
+      </c>
+      <c r="GV12" s="2">
+        <f t="shared" si="53"/>
+        <v>0.95968958707620799</v>
       </c>
     </row>
-    <row r="13" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4" t="s">
         <v>284</v>
       </c>
@@ -7136,7 +7198,7 @@
         <v>0.7</v>
       </c>
       <c r="CR13" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="41"/>
         <v>0.10049780070812771</v>
       </c>
       <c r="CS13" s="2">
@@ -7176,7 +7238,7 @@
         <v>1</v>
       </c>
       <c r="DL13" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>0.14096727085301949</v>
       </c>
       <c r="DM13" s="2">
@@ -7186,112 +7248,112 @@
         <v>0.7</v>
       </c>
       <c r="DP13" s="2">
-        <f t="shared" ref="DP13:DP32" si="48">$CC$3*DO13/(1+$CC$3*DO13)</f>
+        <f t="shared" ref="DP13:DP32" si="54">$CC$3*DO13/(1+$CC$3*DO13)</f>
         <v>6.9311187903279087E-2</v>
       </c>
       <c r="DQ13" s="2">
         <v>0.91</v>
       </c>
       <c r="DR13">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.97731054704451703</v>
       </c>
       <c r="DT13" s="2">
         <v>0.7</v>
       </c>
       <c r="DU13" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>7.8942035980208311E-2</v>
       </c>
       <c r="DV13" s="2">
         <v>1.0285</v>
       </c>
       <c r="DW13">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.97439406754034741</v>
       </c>
       <c r="DY13" s="2">
         <v>0.7</v>
       </c>
       <c r="DZ13" s="2">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v>7.9007354126277282E-2</v>
       </c>
       <c r="EA13" s="2">
         <v>0.80169999999999997</v>
       </c>
       <c r="EB13">
-        <f t="shared" si="26"/>
+        <f t="shared" si="25"/>
         <v>0.97998362178217957</v>
       </c>
       <c r="ED13" s="2">
         <v>7.9809999999999999</v>
       </c>
       <c r="EE13" s="2">
-        <f t="shared" si="27"/>
+        <f t="shared" si="26"/>
         <v>0.45090096142793945</v>
       </c>
       <c r="EF13" s="2">
         <v>1.7</v>
       </c>
       <c r="EG13">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>0.61333865086347206</v>
       </c>
       <c r="EI13" s="2">
         <v>5.0730000000000004</v>
       </c>
       <c r="EJ13" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.43194469354458598</v>
       </c>
       <c r="EK13" s="2">
         <v>1.47</v>
       </c>
       <c r="EL13">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.76438516020631775</v>
       </c>
       <c r="EN13" s="2">
         <v>4.3490000000000002</v>
       </c>
       <c r="EO13" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>0.34103487836492302</v>
       </c>
       <c r="EP13" s="2">
         <v>1.17</v>
       </c>
       <c r="EQ13">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>0.83249321211796445</v>
       </c>
       <c r="ES13" s="2">
         <v>6.9489999999999998</v>
       </c>
       <c r="ET13" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="32"/>
         <v>0.45660238642408441</v>
       </c>
       <c r="EU13" s="2">
         <v>1.19</v>
       </c>
       <c r="EV13">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>0.74234627233627271</v>
       </c>
       <c r="EX13" s="2">
         <v>5.8879999999999999</v>
       </c>
       <c r="EY13" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.5561523393115233</v>
       </c>
       <c r="EZ13" s="2">
         <v>0.78</v>
       </c>
       <c r="FA13">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.84749467240479803</v>
       </c>
       <c r="FF13"/>
@@ -7299,84 +7361,96 @@
         <v>3.3759999999999999</v>
       </c>
       <c r="FI13" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.40292399107767829</v>
       </c>
       <c r="FJ13" s="2">
         <v>2.21</v>
       </c>
-      <c r="FK13" s="2">
-        <f t="shared" si="38"/>
-        <v>0.76428464417717057</v>
+      <c r="FK13">
+        <f t="shared" si="43"/>
+        <v>0.66816342815893837</v>
       </c>
       <c r="FR13" s="2">
         <v>2.2130000000000001</v>
       </c>
       <c r="FS13" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>0.25971269345992959</v>
       </c>
       <c r="FT13" s="2">
         <v>1.39</v>
       </c>
-      <c r="FU13" s="2">
-        <f t="shared" si="40"/>
-        <v>0.89509143840689942</v>
+      <c r="FU13">
+        <f t="shared" si="45"/>
+        <v>0.84683949529982472</v>
       </c>
       <c r="FW13" s="2">
         <v>2.395</v>
       </c>
       <c r="FX13" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>0.37209391327618574</v>
       </c>
       <c r="FY13" s="2">
         <v>1.62</v>
       </c>
-      <c r="FZ13" s="2">
-        <f t="shared" si="42"/>
-        <v>0.86953992535188906</v>
+      <c r="FZ13">
+        <f t="shared" si="46"/>
+        <v>0.81083836913062435</v>
       </c>
       <c r="GB13" s="2">
         <v>2.9329999999999998</v>
       </c>
       <c r="GC13" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="39"/>
         <v>0.50035329768497339</v>
       </c>
       <c r="GD13" s="2">
         <v>1.96</v>
       </c>
-      <c r="GE13" s="2">
-        <f t="shared" si="44"/>
-        <v>0.81292020725998193</v>
+      <c r="GE13">
+        <f t="shared" si="47"/>
+        <v>0.7329458308398954</v>
       </c>
       <c r="GL13" s="2">
         <v>2.2450000000000001</v>
       </c>
       <c r="GM13" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0.40014851123158923</v>
       </c>
       <c r="GN13" s="2">
         <v>1.37</v>
       </c>
-      <c r="GO13" s="2">
-        <f t="shared" si="46"/>
-        <v>0.89510498339874134</v>
+      <c r="GO13">
+        <f t="shared" si="49"/>
+        <v>0.8468587175998441</v>
       </c>
       <c r="GQ13" s="2">
-        <f>(1/GR12)/BH3</f>
-        <v>19.141137174959567</v>
+        <f t="shared" si="50"/>
+        <v>6.9386622259228421</v>
       </c>
       <c r="GR13" s="2">
-        <v>2.8</v>
+        <v>8</v>
       </c>
       <c r="GS13" s="2">
-        <v>0.67600000000000005</v>
+        <f t="shared" si="51"/>
+        <v>0.3570749856131476</v>
+      </c>
+      <c r="GT13" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="GU13" s="2">
+        <f t="shared" si="52"/>
+        <v>0.88889013825755647</v>
+      </c>
+      <c r="GV13" s="2">
+        <f t="shared" si="53"/>
+        <v>0.95624865595450215</v>
       </c>
     </row>
-    <row r="14" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4" t="s">
         <v>290</v>
       </c>
@@ -7581,7 +7655,7 @@
         <v>0.8</v>
       </c>
       <c r="CR14" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="41"/>
         <v>0.11322901974349477</v>
       </c>
       <c r="CS14" s="2">
@@ -7621,7 +7695,7 @@
         <v>1.5</v>
       </c>
       <c r="DL14" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>0.19752838743329451</v>
       </c>
       <c r="DM14" s="2">
@@ -7631,28 +7705,28 @@
         <v>0.8</v>
       </c>
       <c r="DP14" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>7.843614299722057E-2</v>
       </c>
       <c r="DQ14" s="2">
         <v>0.91100000000000003</v>
       </c>
       <c r="DR14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.97408342034845929</v>
       </c>
       <c r="DT14" s="2">
         <v>0.8</v>
       </c>
       <c r="DU14" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>8.9213371804960501E-2</v>
       </c>
       <c r="DV14" s="2">
         <v>0.91100000000000003</v>
       </c>
       <c r="DW14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.97408342034845929</v>
       </c>
       <c r="EB14"/>
@@ -7660,98 +7734,110 @@
         <v>6.6929999999999996</v>
       </c>
       <c r="EJ14" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.50080215353152246</v>
       </c>
       <c r="EK14" s="2">
         <v>1.66</v>
       </c>
       <c r="EL14" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.67011768847610276</v>
       </c>
       <c r="FH14" s="2">
         <v>3.9489999999999998</v>
       </c>
       <c r="FI14" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.44114271873147265</v>
       </c>
       <c r="FJ14" s="2">
         <v>2.4500000000000002</v>
       </c>
-      <c r="FK14" s="2">
-        <f t="shared" si="38"/>
-        <v>0.70568406484515256</v>
+      <c r="FK14">
+        <f t="shared" si="43"/>
+        <v>0.59280992485969486</v>
       </c>
       <c r="FR14" s="2">
         <v>2.6930000000000001</v>
       </c>
       <c r="FS14" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>0.29919049704556583</v>
       </c>
       <c r="FT14" s="2">
         <v>1.54</v>
       </c>
-      <c r="FU14" s="2">
-        <f t="shared" si="40"/>
-        <v>0.86120522499020669</v>
+      <c r="FU14">
+        <f t="shared" si="45"/>
+        <v>0.79920829736841181</v>
       </c>
       <c r="FW14" s="2">
         <v>2.6560000000000001</v>
       </c>
       <c r="FX14" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>0.39656309372157211</v>
       </c>
       <c r="FY14" s="2">
         <v>1.81</v>
       </c>
-      <c r="FZ14" s="2">
-        <f t="shared" si="42"/>
-        <v>0.8409635260134265</v>
+      <c r="FZ14">
+        <f t="shared" si="46"/>
+        <v>0.77119772580275148</v>
       </c>
       <c r="GB14" s="2">
         <v>3.5169999999999999</v>
       </c>
       <c r="GC14" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="39"/>
         <v>0.54562169677481054</v>
       </c>
       <c r="GD14" s="2">
         <v>2.2599999999999998</v>
       </c>
-      <c r="GE14" s="2">
-        <f t="shared" si="44"/>
-        <v>0.75097872995281467</v>
+      <c r="GE14">
+        <f t="shared" si="47"/>
+        <v>0.65079087504023392</v>
       </c>
       <c r="GL14" s="2">
         <v>2.5030000000000001</v>
       </c>
       <c r="GM14" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0.42652047572512208</v>
       </c>
       <c r="GN14" s="2">
         <v>1.42</v>
       </c>
-      <c r="GO14" s="2">
-        <f t="shared" si="46"/>
-        <v>0.87980202548305697</v>
+      <c r="GO14">
+        <f t="shared" si="49"/>
+        <v>0.82523461455903513</v>
       </c>
       <c r="GQ14" s="2">
-        <f>(1/GR13)/BH3</f>
-        <v>19.824749216922406</v>
+        <f t="shared" si="50"/>
+        <v>8.1631320304974615</v>
       </c>
       <c r="GR14" s="2">
-        <v>2.7</v>
+        <v>6.8</v>
       </c>
       <c r="GS14" s="2">
-        <v>0.66500000000000004</v>
+        <f t="shared" si="51"/>
+        <v>0.39518625490631709</v>
+      </c>
+      <c r="GT14" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="GU14" s="2">
+        <f t="shared" si="52"/>
+        <v>0.87179628565173184</v>
+      </c>
+      <c r="GV14" s="2">
+        <f t="shared" si="53"/>
+        <v>0.95205727950482599</v>
       </c>
     </row>
-    <row r="15" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4" t="s">
         <v>297</v>
       </c>
@@ -7953,7 +8039,7 @@
         <v>0.9</v>
       </c>
       <c r="CR15" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="41"/>
         <v>0.12560488249642324</v>
       </c>
       <c r="CS15" s="2">
@@ -7993,7 +8079,7 @@
         <v>2</v>
       </c>
       <c r="DL15" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>0.24710134015961449</v>
       </c>
       <c r="DM15" s="2">
@@ -8003,28 +8089,28 @@
         <v>0.9</v>
       </c>
       <c r="DP15" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>8.7383903824865328E-2</v>
       </c>
       <c r="DQ15" s="2">
         <v>0.91220000000000001</v>
       </c>
       <c r="DR15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.97085365751222485</v>
       </c>
       <c r="DT15" s="2">
         <v>0.9</v>
       </c>
       <c r="DU15" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>9.9258149011525895E-2</v>
       </c>
       <c r="DV15" s="2">
         <v>0.91220000000000001</v>
       </c>
       <c r="DW15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.97085365751222485</v>
       </c>
       <c r="EB15"/>
@@ -8032,98 +8118,110 @@
         <v>8.3979999999999997</v>
       </c>
       <c r="EJ15" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>0.55728239426922954</v>
       </c>
       <c r="EK15" s="2">
         <v>1.8</v>
       </c>
       <c r="EL15" s="2">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>0.58005230275597131</v>
       </c>
       <c r="FH15" s="2">
         <v>4.5960000000000001</v>
       </c>
       <c r="FI15" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.47881226986825476</v>
       </c>
       <c r="FJ15" s="2">
         <v>2.7</v>
       </c>
-      <c r="FK15" s="2">
-        <f t="shared" si="38"/>
-        <v>0.63948135101347503</v>
+      <c r="FK15">
+        <f t="shared" si="43"/>
+        <v>0.51137774732544228</v>
       </c>
       <c r="FR15" s="2">
         <v>3.2029999999999998</v>
       </c>
       <c r="FS15" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>0.33676956998506646</v>
       </c>
       <c r="FT15" s="2">
         <v>1.87</v>
       </c>
-      <c r="FU15" s="2">
-        <f t="shared" si="40"/>
-        <v>0.80589411313039805</v>
+      <c r="FU15">
+        <f t="shared" si="45"/>
+        <v>0.72346408296627762</v>
       </c>
       <c r="FW15" s="2">
         <v>3.34</v>
       </c>
       <c r="FX15" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="38"/>
         <v>0.45247967029639791</v>
       </c>
       <c r="FY15" s="2">
         <v>2.09</v>
       </c>
-      <c r="FZ15" s="2">
-        <f t="shared" si="42"/>
-        <v>0.7776273637667005</v>
+      <c r="FZ15">
+        <f t="shared" si="46"/>
+        <v>0.68573655567773595</v>
       </c>
       <c r="GB15" s="2">
         <v>4.1559999999999997</v>
       </c>
       <c r="GC15" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="39"/>
         <v>0.58660314399553382</v>
       </c>
       <c r="GD15" s="2">
         <v>2.59</v>
       </c>
-      <c r="GE15" s="2">
-        <f t="shared" si="44"/>
-        <v>0.6785321239859966</v>
+      <c r="GE15">
+        <f t="shared" si="47"/>
+        <v>0.55892768292238448</v>
       </c>
       <c r="GL15" s="2">
         <v>3.3980000000000001</v>
       </c>
       <c r="GM15" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="40"/>
         <v>0.50240876948415492</v>
       </c>
       <c r="GN15" s="2">
         <v>1.6</v>
       </c>
-      <c r="GO15" s="2">
-        <f t="shared" si="46"/>
-        <v>0.82210642126294919</v>
+      <c r="GO15">
+        <f t="shared" si="49"/>
+        <v>0.74540458635814377</v>
       </c>
       <c r="GQ15" s="2">
-        <f>(1/GR14)/BH3</f>
-        <v>20.558999187919532</v>
+        <f t="shared" si="50"/>
+        <v>9.3292937491399552</v>
       </c>
       <c r="GR15" s="2">
-        <v>2.6</v>
+        <v>5.95</v>
       </c>
       <c r="GS15" s="2">
-        <v>0.65400000000000003</v>
+        <f t="shared" si="51"/>
+        <v>0.4275064792523724</v>
+      </c>
+      <c r="GT15" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="GU15" s="2">
+        <f t="shared" si="52"/>
+        <v>0.85611666614947202</v>
+      </c>
+      <c r="GV15" s="2">
+        <f t="shared" si="53"/>
+        <v>0.9461327317024566</v>
       </c>
     </row>
-    <row r="16" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4" t="s">
         <v>304</v>
       </c>
@@ -8312,7 +8410,7 @@
         <v>1</v>
       </c>
       <c r="CR16" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="41"/>
         <v>0.13764006234517406</v>
       </c>
       <c r="CS16" s="2">
@@ -8352,7 +8450,7 @@
         <v>2.5</v>
       </c>
       <c r="DL16" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>0.29090586775394434</v>
       </c>
       <c r="DM16" s="2">
@@ -8362,43 +8460,55 @@
         <v>1</v>
       </c>
       <c r="DP16" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>9.6159582064190743E-2</v>
       </c>
       <c r="DQ16" s="2">
         <v>0.91349999999999998</v>
       </c>
       <c r="DR16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.96762275008731913</v>
       </c>
       <c r="DT16" s="2">
         <v>1</v>
       </c>
       <c r="DU16" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.10908378176116316</v>
       </c>
       <c r="DV16" s="2">
         <v>0.91349999999999998</v>
       </c>
       <c r="DW16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.96762275008731913</v>
       </c>
       <c r="EB16"/>
       <c r="GQ16" s="2">
-        <f>(1/GR15)/BH3</f>
-        <v>21.349729925916435</v>
+        <f t="shared" si="50"/>
+        <v>10.674864962958218</v>
       </c>
       <c r="GR16" s="2">
-        <v>2.5</v>
+        <v>5.2</v>
       </c>
       <c r="GS16" s="2">
-        <v>0.64500000000000002</v>
+        <f t="shared" si="51"/>
+        <v>0.46075603985701208</v>
+      </c>
+      <c r="GT16" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="GU16" s="2">
+        <f t="shared" si="52"/>
+        <v>0.83871138863949279</v>
+      </c>
+      <c r="GV16" s="2">
+        <f t="shared" si="53"/>
+        <v>0.9419211551204647</v>
       </c>
     </row>
-    <row r="17" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4" t="s">
         <v>312</v>
       </c>
@@ -8590,7 +8700,7 @@
         <v>1.2</v>
       </c>
       <c r="CR17" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="41"/>
         <v>0.16074313576846283</v>
       </c>
       <c r="CS17" s="2">
@@ -8630,7 +8740,7 @@
         <v>3</v>
       </c>
       <c r="DL17" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>0.32989345305903639</v>
       </c>
       <c r="DM17" s="2">
@@ -8640,43 +8750,55 @@
         <v>1.2</v>
       </c>
       <c r="DP17" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.11321417296580201</v>
       </c>
       <c r="DQ17" s="2">
         <v>0.91659999999999997</v>
       </c>
       <c r="DR17">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.96114536582444166</v>
       </c>
       <c r="DT17" s="2">
         <v>1.2</v>
       </c>
       <c r="DU17" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.12810568754097901</v>
       </c>
       <c r="DV17" s="2">
         <v>0.91659999999999997</v>
       </c>
       <c r="DW17">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.96114536582444166</v>
       </c>
       <c r="EB17"/>
       <c r="GQ17" s="2">
-        <f>(1/GR16)/BH3</f>
-        <v>22.203719122953096</v>
+        <f t="shared" si="50"/>
+        <v>11.937483399437147</v>
       </c>
       <c r="GR17" s="2">
-        <v>2.4</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="GS17" s="2">
-        <v>0.629</v>
+        <f t="shared" si="51"/>
+        <v>0.48862496966811186</v>
+      </c>
+      <c r="GT17" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="GU17" s="2">
+        <f t="shared" si="52"/>
+        <v>0.82301069220416956</v>
+      </c>
+      <c r="GV17" s="2">
+        <f t="shared" si="53"/>
+        <v>0.93558930314477762</v>
       </c>
     </row>
-    <row r="18" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="V18" s="2">
         <v>5</v>
       </c>
@@ -8846,7 +8968,7 @@
         <v>1.4</v>
       </c>
       <c r="CR18" s="2">
-        <f t="shared" si="47"/>
+        <f t="shared" si="41"/>
         <v>0.18264062071448259</v>
       </c>
       <c r="CS18" s="2">
@@ -8886,7 +9008,7 @@
         <v>3.5</v>
       </c>
       <c r="DL18" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>0.36481722615682666</v>
       </c>
       <c r="DM18" s="2">
@@ -8896,43 +9018,55 @@
         <v>1.4</v>
       </c>
       <c r="DP18" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.12963707606797881</v>
       </c>
       <c r="DQ18" s="2">
         <v>0.92020000000000002</v>
       </c>
       <c r="DR18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.95464461253083843</v>
       </c>
       <c r="DT18" s="2">
         <v>1.4</v>
       </c>
       <c r="DU18" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.14633230210275425</v>
       </c>
       <c r="DV18" s="2">
         <v>0.92020000000000002</v>
       </c>
       <c r="DW18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.95464461253083843</v>
       </c>
       <c r="EB18"/>
       <c r="GQ18" s="2">
-        <f>(1/GR17)/BH3</f>
-        <v>23.128874086409475</v>
+        <f t="shared" si="50"/>
+        <v>13.705999458613022</v>
       </c>
       <c r="GR18" s="2">
-        <v>2.2999999999999998</v>
+        <v>4.05</v>
       </c>
       <c r="GS18" s="2">
-        <v>0.62</v>
+        <f t="shared" si="51"/>
+        <v>0.52314404058724051</v>
+      </c>
+      <c r="GT18" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="GU18" s="2">
+        <f t="shared" si="52"/>
+        <v>0.80198220692011568</v>
+      </c>
+      <c r="GV18" s="2">
+        <f t="shared" si="53"/>
+        <v>0.93518284262222595</v>
       </c>
     </row>
-    <row r="19" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
         <v>324</v>
       </c>
@@ -9134,7 +9268,7 @@
         <v>4</v>
       </c>
       <c r="DL19" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>0.39628109152378649</v>
       </c>
       <c r="DM19" s="2">
@@ -9144,42 +9278,54 @@
         <v>1.6</v>
       </c>
       <c r="DP19" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.14546274901215495</v>
       </c>
       <c r="DQ19" s="2">
         <v>0.9244</v>
       </c>
       <c r="DR19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.9481058402815703</v>
       </c>
       <c r="DT19" s="2">
         <v>1.6</v>
       </c>
       <c r="DU19" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.1638124799314995</v>
       </c>
       <c r="DV19" s="2">
         <v>0.9244</v>
       </c>
       <c r="DW19">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.9481058402815703</v>
       </c>
       <c r="GQ19" s="2">
-        <f>(1/GR18)/BH3</f>
-        <v>24.134477307557713</v>
+        <f t="shared" si="50"/>
+        <v>15.002512920914251</v>
       </c>
       <c r="GR19" s="2">
-        <v>1.5</v>
+        <v>3.7</v>
       </c>
       <c r="GS19" s="2">
-        <v>0.51900000000000002</v>
+        <f t="shared" si="51"/>
+        <v>0.54562930091309736</v>
+      </c>
+      <c r="GT19" s="2">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="GU19" s="2">
+        <f t="shared" si="52"/>
+        <v>0.78723616136414198</v>
+      </c>
+      <c r="GV19" s="2">
+        <f t="shared" si="53"/>
+        <v>0.92983533522084727</v>
       </c>
     </row>
-    <row r="20" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4" t="s">
         <v>331</v>
       </c>
@@ -9359,7 +9505,7 @@
         <v>4.5</v>
       </c>
       <c r="DL20" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>0.42477494319652565</v>
       </c>
       <c r="DM20" s="2">
@@ -9369,42 +9515,54 @@
         <v>1.8</v>
       </c>
       <c r="DP20" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.16072318804332683</v>
       </c>
       <c r="DQ20" s="2">
         <v>0.92900000000000005</v>
       </c>
       <c r="DR20">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.94153043639048362</v>
       </c>
       <c r="DT20" s="2">
         <v>1.8</v>
       </c>
       <c r="DU20" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.18059115431762909</v>
       </c>
       <c r="DV20" s="2">
         <v>0.92900000000000005</v>
       </c>
       <c r="DW20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.94153043639048362</v>
       </c>
       <c r="GQ20" s="2">
-        <f>(1/GR19)/BH3</f>
-        <v>37.006198538255155</v>
+        <f t="shared" si="50"/>
+        <v>16.326264060994923</v>
       </c>
       <c r="GR20" s="2">
-        <v>0.8</v>
+        <v>3.4</v>
       </c>
       <c r="GS20" s="2">
-        <v>0.39200000000000002</v>
+        <f t="shared" si="51"/>
+        <v>0.56649963905049039</v>
+      </c>
+      <c r="GT20" s="2">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="GU20" s="2">
+        <f t="shared" si="52"/>
+        <v>0.77272949429646598</v>
+      </c>
+      <c r="GV20" s="2">
+        <f t="shared" si="53"/>
+        <v>0.92529145746012187</v>
       </c>
     </row>
-    <row r="21" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4" t="s">
         <v>337</v>
       </c>
@@ -9518,7 +9676,7 @@
         <v>5</v>
       </c>
       <c r="DL21" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>0.45070035704476791</v>
       </c>
       <c r="DM21" s="2">
@@ -9528,42 +9686,54 @@
         <v>2</v>
       </c>
       <c r="DP21" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.17544814393377201</v>
       </c>
       <c r="DQ21" s="2">
         <v>0.93379999999999996</v>
       </c>
       <c r="DR21">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.93492517765215333</v>
       </c>
       <c r="DT21" s="2">
         <v>2</v>
       </c>
       <c r="DU21" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.19670972302551248</v>
       </c>
       <c r="DV21" s="2">
         <v>0.93379999999999996</v>
       </c>
       <c r="DW21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.93492517765215333</v>
       </c>
       <c r="GQ21" s="2">
-        <f>(1/GR20)/BH3</f>
-        <v>69.386622259228417</v>
+        <f t="shared" si="50"/>
+        <v>17.346655564807104</v>
       </c>
       <c r="GR21" s="2">
-        <v>0.5</v>
+        <v>3.2</v>
       </c>
       <c r="GS21" s="2">
-        <v>0.29199999999999998</v>
+        <f t="shared" si="51"/>
+        <v>0.58132339804344513</v>
+      </c>
+      <c r="GT21" s="2">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="GU21" s="2">
+        <f>1-(GQ21/(55.51))/(GQ21/(55.51) +1)</f>
+        <v>0.76190705666722525</v>
+      </c>
+      <c r="GV21" s="2">
+        <f t="shared" si="53"/>
+        <v>0.92662220912905446</v>
       </c>
     </row>
-    <row r="22" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4" t="s">
         <v>341</v>
       </c>
@@ -9687,7 +9857,7 @@
         <v>5.5</v>
       </c>
       <c r="DL22" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>0.47438963496360148</v>
       </c>
       <c r="DM22" s="2">
@@ -9697,32 +9867,54 @@
         <v>2.4</v>
       </c>
       <c r="DP22" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.20340052384381552</v>
       </c>
       <c r="DQ22" s="2">
         <v>0.94450000000000001</v>
       </c>
       <c r="DR22">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.92157439663809559</v>
       </c>
       <c r="DT22" s="2">
         <v>2.4</v>
       </c>
       <c r="DU22" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.22711646427423143</v>
       </c>
       <c r="DV22" s="2">
         <v>0.94450000000000001</v>
       </c>
       <c r="DW22">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.92157439663809559</v>
       </c>
+      <c r="GQ22" s="2">
+        <f t="shared" si="50"/>
+        <v>18.503099269127578</v>
+      </c>
+      <c r="GR22" s="2">
+        <v>3</v>
+      </c>
+      <c r="GS22" s="2">
+        <f>$CS$3*GQ22/(1+$CS$3*GQ22)</f>
+        <v>0.59694379810273845</v>
+      </c>
+      <c r="GT22" s="2">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="GU22" s="2">
+        <f t="shared" si="52"/>
+        <v>0.75000237185249707</v>
+      </c>
+      <c r="GV22" s="2">
+        <f t="shared" si="53"/>
+        <v>0.92933039435384468</v>
+      </c>
     </row>
-    <row r="23" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>350</v>
       </c>
@@ -9839,7 +10031,7 @@
         <v>6</v>
       </c>
       <c r="DL23" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="42"/>
         <v>0.49612012496220897</v>
       </c>
       <c r="DM23" s="2">
@@ -9849,32 +10041,54 @@
         <v>2.7</v>
       </c>
       <c r="DP23" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.22315193672106418</v>
       </c>
       <c r="DQ23" s="2">
         <v>0.95279999999999998</v>
       </c>
       <c r="DR23">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.91147768727147049</v>
       </c>
       <c r="DT23" s="2">
         <v>2.7</v>
       </c>
       <c r="DU23" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.24845256382892372</v>
       </c>
       <c r="DV23" s="2">
         <v>0.95279999999999998</v>
       </c>
       <c r="DW23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.91147768727147049</v>
       </c>
+      <c r="GQ23" s="2">
+        <f t="shared" si="50"/>
+        <v>19.141137174959567</v>
+      </c>
+      <c r="GR23" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="GS23" s="2">
+        <f t="shared" si="51"/>
+        <v>0.60507308001950311</v>
+      </c>
+      <c r="GT23" s="2">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="GU23" s="2">
+        <f t="shared" si="52"/>
+        <v>0.74359215546712221</v>
+      </c>
+      <c r="GV23" s="2">
+        <f t="shared" si="53"/>
+        <v>0.9225487317964739</v>
+      </c>
     </row>
-    <row r="24" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="9" t="s">
         <v>352</v>
       </c>
@@ -9933,32 +10147,54 @@
         <v>3</v>
       </c>
       <c r="DP24" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.24194758825625207</v>
       </c>
       <c r="DQ24" s="2">
         <v>0.96179999999999999</v>
       </c>
       <c r="DR24">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.90126166538009622</v>
       </c>
       <c r="DT24" s="2">
         <v>3</v>
       </c>
       <c r="DU24" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.26864230757979113</v>
       </c>
       <c r="DV24" s="2">
         <v>0.96179999999999999</v>
       </c>
       <c r="DW24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.90126166538009622</v>
       </c>
+      <c r="GQ24" s="2">
+        <f t="shared" si="50"/>
+        <v>19.824749216922406</v>
+      </c>
+      <c r="GR24" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="GS24" s="2">
+        <f t="shared" si="51"/>
+        <v>0.61342683067019199</v>
+      </c>
+      <c r="GT24" s="2">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="GU24" s="2">
+        <f t="shared" si="52"/>
+        <v>0.73684455814888161</v>
+      </c>
+      <c r="GV24" s="2">
+        <f t="shared" si="53"/>
+        <v>0.91742551739577649</v>
+      </c>
     </row>
-    <row r="25" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
         <v>383</v>
       </c>
@@ -10007,32 +10243,54 @@
         <v>3.4</v>
       </c>
       <c r="DP25" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.26563787428601643</v>
       </c>
       <c r="DQ25" s="2">
         <v>0.97419999999999995</v>
       </c>
       <c r="DR25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.88750605177911046</v>
       </c>
       <c r="DT25" s="2">
         <v>3.4</v>
       </c>
       <c r="DU25" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.29393290668052435</v>
       </c>
       <c r="DV25" s="2">
         <v>0.97419999999999995</v>
       </c>
       <c r="DW25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.88750605177911046</v>
       </c>
+      <c r="GQ25" s="2">
+        <f t="shared" si="50"/>
+        <v>20.558999187919532</v>
+      </c>
+      <c r="GR25" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="GS25" s="2">
+        <f t="shared" si="51"/>
+        <v>0.62201447738054993</v>
+      </c>
+      <c r="GT25" s="2">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="GU25" s="2">
+        <f>1-(GQ25/(55.51))/(GQ25/(55.51) +1)</f>
+        <v>0.72973222459347808</v>
+      </c>
+      <c r="GV25" s="2">
+        <f t="shared" si="53"/>
+        <v>0.91129318068756071</v>
+      </c>
     </row>
-    <row r="26" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX26" s="2">
         <v>7.4950000000000001</v>
       </c>
@@ -10059,32 +10317,54 @@
         <v>3.7</v>
       </c>
       <c r="DP26" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.28245612398584147</v>
       </c>
       <c r="DQ26" s="2">
         <v>0.98360000000000003</v>
       </c>
       <c r="DR26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.87710984737211428</v>
       </c>
       <c r="DT26" s="2">
         <v>3.7</v>
       </c>
       <c r="DU26" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.31178201658880628</v>
       </c>
       <c r="DV26" s="2">
         <v>0.98360000000000003</v>
       </c>
       <c r="DW26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.87710984737211428</v>
       </c>
+      <c r="GQ26" s="2">
+        <f t="shared" si="50"/>
+        <v>21.349729925916435</v>
+      </c>
+      <c r="GR26" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="GS26" s="2">
+        <f t="shared" si="51"/>
+        <v>0.63084598288173266</v>
+      </c>
+      <c r="GT26" s="2">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="GU26" s="2">
+        <f t="shared" si="52"/>
+        <v>0.72222476000767877</v>
+      </c>
+      <c r="GV26" s="2">
+        <f t="shared" si="53"/>
+        <v>0.90553527961717439</v>
+      </c>
     </row>
-    <row r="27" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX27" s="2">
         <v>7.9480000000000004</v>
       </c>
@@ -10111,32 +10391,54 @@
         <v>4</v>
       </c>
       <c r="DP27" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.29852128286427793</v>
       </c>
       <c r="DQ27" s="2">
         <v>0.99250000000000005</v>
       </c>
       <c r="DR27">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.8667217477376794</v>
       </c>
       <c r="DT27" s="2">
         <v>4</v>
       </c>
       <c r="DU27" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.32875093974868436</v>
       </c>
       <c r="DV27" s="2">
         <v>0.99250000000000005</v>
       </c>
       <c r="DW27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.8667217477376794</v>
       </c>
+      <c r="GQ27" s="2">
+        <f t="shared" si="50"/>
+        <v>22.203719122953096</v>
+      </c>
+      <c r="GR27" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="GS27" s="2">
+        <f t="shared" si="51"/>
+        <v>0.63993188386678979</v>
+      </c>
+      <c r="GT27" s="2">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="GU27" s="2">
+        <f t="shared" si="52"/>
+        <v>0.71428829589504061</v>
+      </c>
+      <c r="GV27" s="2">
+        <f t="shared" si="53"/>
+        <v>0.90299673634128541</v>
+      </c>
     </row>
-    <row r="28" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX28" s="2">
         <v>7.9969999999999999</v>
       </c>
@@ -10163,32 +10465,54 @@
         <v>4.5</v>
       </c>
       <c r="DP28" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.32375545644816078</v>
       </c>
       <c r="DQ28" s="2">
         <v>1.0089999999999999</v>
       </c>
       <c r="DR28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.8490882556844872</v>
       </c>
       <c r="DT28" s="2">
         <v>4.5</v>
       </c>
       <c r="DU28" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.35524636036570428</v>
       </c>
       <c r="DV28" s="2">
         <v>1.0089999999999999</v>
       </c>
       <c r="DW28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.8490882556844872</v>
       </c>
+      <c r="GQ28" s="2">
+        <f t="shared" si="50"/>
+        <v>23.128874086409475</v>
+      </c>
+      <c r="GR28" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="GS28" s="2">
+        <f t="shared" si="51"/>
+        <v>0.64928333292774931</v>
+      </c>
+      <c r="GT28" s="2">
+        <v>0.629</v>
+      </c>
+      <c r="GU28" s="2">
+        <f t="shared" si="52"/>
+        <v>0.70588497921530324</v>
+      </c>
+      <c r="GV28" s="2">
+        <f t="shared" si="53"/>
+        <v>0.89108001802110537</v>
+      </c>
     </row>
-    <row r="29" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX29" s="2">
         <v>8.9870000000000001</v>
       </c>
@@ -10215,32 +10539,54 @@
         <v>5</v>
       </c>
       <c r="DP29" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.34723718137014914</v>
       </c>
       <c r="DQ29" s="2">
         <v>1.0249999999999999</v>
       </c>
       <c r="DR29">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.83139404553783947</v>
       </c>
       <c r="DT29" s="2">
         <v>5</v>
       </c>
       <c r="DU29" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.37972956208907077</v>
       </c>
       <c r="DV29" s="2">
         <v>1.0249999999999999</v>
       </c>
       <c r="DW29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.83139404553783947</v>
       </c>
+      <c r="GQ29" s="2">
+        <f t="shared" si="50"/>
+        <v>24.134477307557713</v>
+      </c>
+      <c r="GR29" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="GS29" s="2">
+        <f t="shared" si="51"/>
+        <v>0.65891214422423905</v>
+      </c>
+      <c r="GT29" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="GU29" s="2">
+        <f>1-(GQ29/(55.51))/(GQ29/(55.51) +1)</f>
+        <v>0.69697236866331325</v>
+      </c>
+      <c r="GV29" s="2">
+        <f t="shared" si="53"/>
+        <v>0.88956180743444035</v>
+      </c>
     </row>
-    <row r="30" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX30" s="2">
         <v>9.9670000000000005</v>
       </c>
@@ -10267,32 +10613,32 @@
         <v>5.5</v>
       </c>
       <c r="DP30" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.36914288598203948</v>
       </c>
       <c r="DQ30" s="2">
         <v>1.0411999999999999</v>
       </c>
       <c r="DR30">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.81356716887718761</v>
       </c>
       <c r="DT30" s="2">
         <v>5.5</v>
       </c>
       <c r="DU30" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.40242138853366155</v>
       </c>
       <c r="DV30" s="2">
         <v>1.0411999999999999</v>
       </c>
       <c r="DW30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.81356716887718761</v>
       </c>
     </row>
-    <row r="31" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX31" s="2">
         <v>11.013</v>
       </c>
@@ -10319,32 +10665,32 @@
         <v>6</v>
       </c>
       <c r="DP31" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.38962608493963408</v>
       </c>
       <c r="DQ31" s="2">
         <v>1.0569999999999999</v>
       </c>
       <c r="DR31">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.79572679892361964</v>
       </c>
       <c r="DT31" s="2">
         <v>6</v>
       </c>
       <c r="DU31" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.42351150671032606</v>
       </c>
       <c r="DV31" s="2">
         <v>1.0569999999999999</v>
       </c>
       <c r="DW31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.79572679892361964</v>
       </c>
     </row>
-    <row r="32" spans="1:201" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:204" ht="49" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AX32" s="2">
         <v>11.999000000000001</v>
       </c>
@@ -10371,28 +10717,28 @@
         <v>6.5</v>
       </c>
       <c r="DP32" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="54"/>
         <v>0.40882098212570239</v>
       </c>
       <c r="DQ32" s="2">
         <v>1.0745</v>
       </c>
       <c r="DR32">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>0.77752510639851602</v>
       </c>
       <c r="DT32" s="2">
         <v>6.5</v>
       </c>
       <c r="DU32" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.44316372100275075</v>
       </c>
       <c r="DV32" s="2">
         <v>1.0745</v>
       </c>
       <c r="DW32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.77752510639851602</v>
       </c>
     </row>

</xml_diff>